<commit_message>
Updated LoCoMo and OpenRave Results file added
</commit_message>
<xml_diff>
--- a/Grasp_Benchmark_LoCoMo.xlsx
+++ b/Grasp_Benchmark_LoCoMo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Grasping_Benchmarking\Benchmark_Results\Grasping_Benchmark_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364F6D8D-10A6-4048-BEBE-495903E3323A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA9D0F3-A34C-43ED-8610-1D04728F5ECE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{CC49EE9F-3C2E-4A23-8A10-0204FB2D8797}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{CC49EE9F-3C2E-4A23-8A10-0204FB2D8797}"/>
   </bookViews>
   <sheets>
     <sheet name="single objects" sheetId="2" r:id="rId1"/>
@@ -619,7 +619,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="453">
   <si>
     <t>Shape complexity</t>
   </si>
@@ -2761,6 +2761,159 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2773,28 +2926,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2806,18 +2971,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2844,159 +2997,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3321,7 +3321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDF97CE-52BF-4919-8890-4F4D9BF946D9}">
   <dimension ref="A1:CA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3344,102 +3344,102 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="154" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="102" t="s">
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="153" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="102" t="s">
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="154"/>
+      <c r="P1" s="155"/>
+      <c r="Q1" s="153" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="103"/>
-      <c r="S1" s="103"/>
-      <c r="T1" s="103"/>
-      <c r="U1" s="103"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="102" t="s">
+      <c r="R1" s="154"/>
+      <c r="S1" s="154"/>
+      <c r="T1" s="154"/>
+      <c r="U1" s="154"/>
+      <c r="V1" s="155"/>
+      <c r="W1" s="153" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="103"/>
-      <c r="Y1" s="103"/>
-      <c r="Z1" s="103"/>
-      <c r="AA1" s="103"/>
-      <c r="AB1" s="104"/>
-      <c r="AC1" s="102" t="s">
+      <c r="X1" s="154"/>
+      <c r="Y1" s="154"/>
+      <c r="Z1" s="154"/>
+      <c r="AA1" s="154"/>
+      <c r="AB1" s="155"/>
+      <c r="AC1" s="153" t="s">
         <v>448</v>
       </c>
-      <c r="AD1" s="103"/>
-      <c r="AE1" s="103"/>
-      <c r="AF1" s="103"/>
-      <c r="AG1" s="103"/>
-      <c r="AH1" s="104"/>
-      <c r="AI1" s="102" t="s">
+      <c r="AD1" s="154"/>
+      <c r="AE1" s="154"/>
+      <c r="AF1" s="154"/>
+      <c r="AG1" s="154"/>
+      <c r="AH1" s="155"/>
+      <c r="AI1" s="153" t="s">
         <v>449</v>
       </c>
-      <c r="AJ1" s="103"/>
-      <c r="AK1" s="103"/>
-      <c r="AL1" s="103"/>
-      <c r="AM1" s="103"/>
-      <c r="AN1" s="104"/>
-      <c r="AO1" s="103" t="s">
+      <c r="AJ1" s="154"/>
+      <c r="AK1" s="154"/>
+      <c r="AL1" s="154"/>
+      <c r="AM1" s="154"/>
+      <c r="AN1" s="155"/>
+      <c r="AO1" s="154" t="s">
         <v>51</v>
       </c>
-      <c r="AP1" s="103"/>
-      <c r="AQ1" s="103"/>
-      <c r="AR1" s="103"/>
-      <c r="AS1" s="103"/>
-      <c r="AT1" s="104"/>
-      <c r="AU1" s="102" t="s">
+      <c r="AP1" s="154"/>
+      <c r="AQ1" s="154"/>
+      <c r="AR1" s="154"/>
+      <c r="AS1" s="154"/>
+      <c r="AT1" s="155"/>
+      <c r="AU1" s="153" t="s">
         <v>52</v>
       </c>
-      <c r="AV1" s="103"/>
-      <c r="AW1" s="103"/>
-      <c r="AX1" s="103"/>
-      <c r="AY1" s="103"/>
-      <c r="AZ1" s="104"/>
-      <c r="BA1" s="102" t="s">
+      <c r="AV1" s="154"/>
+      <c r="AW1" s="154"/>
+      <c r="AX1" s="154"/>
+      <c r="AY1" s="154"/>
+      <c r="AZ1" s="155"/>
+      <c r="BA1" s="153" t="s">
         <v>53</v>
       </c>
-      <c r="BB1" s="103"/>
-      <c r="BC1" s="103"/>
-      <c r="BD1" s="103"/>
-      <c r="BE1" s="103"/>
-      <c r="BF1" s="104"/>
-      <c r="BG1" s="102" t="s">
+      <c r="BB1" s="154"/>
+      <c r="BC1" s="154"/>
+      <c r="BD1" s="154"/>
+      <c r="BE1" s="154"/>
+      <c r="BF1" s="155"/>
+      <c r="BG1" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="BH1" s="103"/>
-      <c r="BI1" s="103"/>
-      <c r="BJ1" s="103"/>
-      <c r="BK1" s="103"/>
-      <c r="BL1" s="104"/>
-      <c r="BM1" s="102" t="s">
+      <c r="BH1" s="154"/>
+      <c r="BI1" s="154"/>
+      <c r="BJ1" s="154"/>
+      <c r="BK1" s="154"/>
+      <c r="BL1" s="155"/>
+      <c r="BM1" s="153" t="s">
         <v>55</v>
       </c>
-      <c r="BN1" s="103"/>
-      <c r="BO1" s="103"/>
-      <c r="BP1" s="103"/>
-      <c r="BQ1" s="103"/>
-      <c r="BR1" s="104"/>
-      <c r="BS1" s="102" t="s">
+      <c r="BN1" s="154"/>
+      <c r="BO1" s="154"/>
+      <c r="BP1" s="154"/>
+      <c r="BQ1" s="154"/>
+      <c r="BR1" s="155"/>
+      <c r="BS1" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="BT1" s="103"/>
-      <c r="BU1" s="103"/>
-      <c r="BV1" s="103"/>
-      <c r="BW1" s="103"/>
-      <c r="BX1" s="104"/>
+      <c r="BT1" s="154"/>
+      <c r="BU1" s="154"/>
+      <c r="BV1" s="154"/>
+      <c r="BW1" s="154"/>
+      <c r="BX1" s="155"/>
     </row>
     <row r="2" spans="1:76" s="4" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="99" t="s">
@@ -3670,13 +3670,13 @@
       </c>
     </row>
     <row r="3" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="163" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="158" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="45">
@@ -3754,59 +3754,59 @@
       <c r="AB3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="130"/>
-      <c r="AD3" s="131"/>
-      <c r="AE3" s="132"/>
-      <c r="AF3" s="132"/>
-      <c r="AG3" s="132"/>
-      <c r="AH3" s="133"/>
-      <c r="AI3" s="130"/>
-      <c r="AJ3" s="131"/>
-      <c r="AK3" s="132"/>
-      <c r="AL3" s="132"/>
-      <c r="AM3" s="132"/>
-      <c r="AN3" s="133"/>
-      <c r="AO3" s="131"/>
-      <c r="AP3" s="132"/>
-      <c r="AQ3" s="132"/>
-      <c r="AR3" s="132"/>
-      <c r="AS3" s="132"/>
-      <c r="AT3" s="133"/>
-      <c r="AU3" s="130"/>
-      <c r="AV3" s="131"/>
-      <c r="AW3" s="132"/>
-      <c r="AX3" s="132"/>
-      <c r="AY3" s="132"/>
-      <c r="AZ3" s="133"/>
-      <c r="BA3" s="130"/>
-      <c r="BB3" s="131"/>
-      <c r="BC3" s="132"/>
-      <c r="BD3" s="132"/>
-      <c r="BE3" s="132"/>
-      <c r="BF3" s="134"/>
-      <c r="BG3" s="130"/>
-      <c r="BH3" s="131"/>
-      <c r="BI3" s="132"/>
-      <c r="BJ3" s="132"/>
-      <c r="BK3" s="132"/>
-      <c r="BL3" s="133"/>
-      <c r="BM3" s="130"/>
-      <c r="BN3" s="131"/>
-      <c r="BO3" s="132"/>
-      <c r="BP3" s="132"/>
-      <c r="BQ3" s="132"/>
-      <c r="BR3" s="133"/>
-      <c r="BS3" s="130"/>
-      <c r="BT3" s="131"/>
-      <c r="BU3" s="132"/>
-      <c r="BV3" s="132"/>
-      <c r="BW3" s="132"/>
-      <c r="BX3" s="133"/>
+      <c r="AC3" s="102"/>
+      <c r="AD3" s="103"/>
+      <c r="AE3" s="104"/>
+      <c r="AF3" s="104"/>
+      <c r="AG3" s="104"/>
+      <c r="AH3" s="105"/>
+      <c r="AI3" s="102"/>
+      <c r="AJ3" s="103"/>
+      <c r="AK3" s="104"/>
+      <c r="AL3" s="104"/>
+      <c r="AM3" s="104"/>
+      <c r="AN3" s="105"/>
+      <c r="AO3" s="103"/>
+      <c r="AP3" s="104"/>
+      <c r="AQ3" s="104"/>
+      <c r="AR3" s="104"/>
+      <c r="AS3" s="104"/>
+      <c r="AT3" s="105"/>
+      <c r="AU3" s="102"/>
+      <c r="AV3" s="103"/>
+      <c r="AW3" s="104"/>
+      <c r="AX3" s="104"/>
+      <c r="AY3" s="104"/>
+      <c r="AZ3" s="105"/>
+      <c r="BA3" s="102"/>
+      <c r="BB3" s="103"/>
+      <c r="BC3" s="104"/>
+      <c r="BD3" s="104"/>
+      <c r="BE3" s="104"/>
+      <c r="BF3" s="106"/>
+      <c r="BG3" s="102"/>
+      <c r="BH3" s="103"/>
+      <c r="BI3" s="104"/>
+      <c r="BJ3" s="104"/>
+      <c r="BK3" s="104"/>
+      <c r="BL3" s="105"/>
+      <c r="BM3" s="102"/>
+      <c r="BN3" s="103"/>
+      <c r="BO3" s="104"/>
+      <c r="BP3" s="104"/>
+      <c r="BQ3" s="104"/>
+      <c r="BR3" s="105"/>
+      <c r="BS3" s="102"/>
+      <c r="BT3" s="103"/>
+      <c r="BU3" s="104"/>
+      <c r="BV3" s="104"/>
+      <c r="BW3" s="104"/>
+      <c r="BX3" s="105"/>
     </row>
     <row r="4" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="105"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="109"/>
+      <c r="A4" s="156"/>
+      <c r="B4" s="167"/>
+      <c r="C4" s="158"/>
       <c r="D4" s="46">
         <v>2</v>
       </c>
@@ -3882,59 +3882,59 @@
       <c r="AB4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AC4" s="135"/>
-      <c r="AD4" s="136"/>
-      <c r="AE4" s="137"/>
-      <c r="AF4" s="137"/>
-      <c r="AG4" s="137"/>
-      <c r="AH4" s="138"/>
-      <c r="AI4" s="135"/>
-      <c r="AJ4" s="136"/>
-      <c r="AK4" s="137"/>
-      <c r="AL4" s="137"/>
-      <c r="AM4" s="137"/>
-      <c r="AN4" s="138"/>
-      <c r="AO4" s="136"/>
-      <c r="AP4" s="139"/>
-      <c r="AQ4" s="140"/>
-      <c r="AR4" s="140"/>
-      <c r="AS4" s="137"/>
-      <c r="AT4" s="138"/>
-      <c r="AU4" s="135"/>
-      <c r="AV4" s="136"/>
-      <c r="AW4" s="137"/>
-      <c r="AX4" s="137"/>
-      <c r="AY4" s="137"/>
-      <c r="AZ4" s="138"/>
-      <c r="BA4" s="135"/>
-      <c r="BB4" s="136"/>
-      <c r="BC4" s="137"/>
-      <c r="BD4" s="137"/>
-      <c r="BE4" s="137"/>
-      <c r="BF4" s="141"/>
-      <c r="BG4" s="135"/>
-      <c r="BH4" s="136"/>
-      <c r="BI4" s="137"/>
-      <c r="BJ4" s="137"/>
-      <c r="BK4" s="137"/>
-      <c r="BL4" s="138"/>
-      <c r="BM4" s="135"/>
-      <c r="BN4" s="136"/>
-      <c r="BO4" s="137"/>
-      <c r="BP4" s="137"/>
-      <c r="BQ4" s="137"/>
-      <c r="BR4" s="138"/>
-      <c r="BS4" s="135"/>
-      <c r="BT4" s="136"/>
-      <c r="BU4" s="137"/>
-      <c r="BV4" s="137"/>
-      <c r="BW4" s="137"/>
-      <c r="BX4" s="138"/>
+      <c r="AC4" s="107"/>
+      <c r="AD4" s="108"/>
+      <c r="AE4" s="109"/>
+      <c r="AF4" s="109"/>
+      <c r="AG4" s="109"/>
+      <c r="AH4" s="110"/>
+      <c r="AI4" s="107"/>
+      <c r="AJ4" s="108"/>
+      <c r="AK4" s="109"/>
+      <c r="AL4" s="109"/>
+      <c r="AM4" s="109"/>
+      <c r="AN4" s="110"/>
+      <c r="AO4" s="108"/>
+      <c r="AP4" s="111"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="112"/>
+      <c r="AS4" s="109"/>
+      <c r="AT4" s="110"/>
+      <c r="AU4" s="107"/>
+      <c r="AV4" s="108"/>
+      <c r="AW4" s="109"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="109"/>
+      <c r="AZ4" s="110"/>
+      <c r="BA4" s="107"/>
+      <c r="BB4" s="108"/>
+      <c r="BC4" s="109"/>
+      <c r="BD4" s="109"/>
+      <c r="BE4" s="109"/>
+      <c r="BF4" s="113"/>
+      <c r="BG4" s="107"/>
+      <c r="BH4" s="108"/>
+      <c r="BI4" s="109"/>
+      <c r="BJ4" s="109"/>
+      <c r="BK4" s="109"/>
+      <c r="BL4" s="110"/>
+      <c r="BM4" s="107"/>
+      <c r="BN4" s="108"/>
+      <c r="BO4" s="109"/>
+      <c r="BP4" s="109"/>
+      <c r="BQ4" s="109"/>
+      <c r="BR4" s="110"/>
+      <c r="BS4" s="107"/>
+      <c r="BT4" s="108"/>
+      <c r="BU4" s="109"/>
+      <c r="BV4" s="109"/>
+      <c r="BW4" s="109"/>
+      <c r="BX4" s="110"/>
     </row>
     <row r="5" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="110"/>
+      <c r="A5" s="156"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="159"/>
       <c r="D5" s="100">
         <v>3</v>
       </c>
@@ -4010,59 +4010,59 @@
       <c r="AB5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="AC5" s="142"/>
-      <c r="AD5" s="143"/>
-      <c r="AE5" s="144"/>
-      <c r="AF5" s="144"/>
-      <c r="AG5" s="144"/>
-      <c r="AH5" s="145"/>
-      <c r="AI5" s="142"/>
-      <c r="AJ5" s="143"/>
-      <c r="AK5" s="144"/>
-      <c r="AL5" s="144"/>
-      <c r="AM5" s="144"/>
-      <c r="AN5" s="145"/>
-      <c r="AO5" s="143"/>
-      <c r="AP5" s="144"/>
-      <c r="AQ5" s="144"/>
-      <c r="AR5" s="144"/>
-      <c r="AS5" s="144"/>
-      <c r="AT5" s="145"/>
-      <c r="AU5" s="142"/>
-      <c r="AV5" s="143"/>
-      <c r="AW5" s="144"/>
-      <c r="AX5" s="144"/>
-      <c r="AY5" s="144"/>
-      <c r="AZ5" s="145"/>
-      <c r="BA5" s="142"/>
-      <c r="BB5" s="143"/>
-      <c r="BC5" s="144"/>
-      <c r="BD5" s="144"/>
-      <c r="BE5" s="144"/>
-      <c r="BF5" s="146"/>
-      <c r="BG5" s="142"/>
-      <c r="BH5" s="143"/>
-      <c r="BI5" s="144"/>
-      <c r="BJ5" s="144"/>
-      <c r="BK5" s="144"/>
-      <c r="BL5" s="145"/>
-      <c r="BM5" s="142"/>
-      <c r="BN5" s="143"/>
-      <c r="BO5" s="144"/>
-      <c r="BP5" s="144"/>
-      <c r="BQ5" s="144"/>
-      <c r="BR5" s="145"/>
-      <c r="BS5" s="142"/>
-      <c r="BT5" s="143"/>
-      <c r="BU5" s="144"/>
-      <c r="BV5" s="144"/>
-      <c r="BW5" s="144"/>
-      <c r="BX5" s="145"/>
+      <c r="AC5" s="114"/>
+      <c r="AD5" s="115"/>
+      <c r="AE5" s="116"/>
+      <c r="AF5" s="116"/>
+      <c r="AG5" s="116"/>
+      <c r="AH5" s="117"/>
+      <c r="AI5" s="114"/>
+      <c r="AJ5" s="115"/>
+      <c r="AK5" s="116"/>
+      <c r="AL5" s="116"/>
+      <c r="AM5" s="116"/>
+      <c r="AN5" s="117"/>
+      <c r="AO5" s="115"/>
+      <c r="AP5" s="116"/>
+      <c r="AQ5" s="116"/>
+      <c r="AR5" s="116"/>
+      <c r="AS5" s="116"/>
+      <c r="AT5" s="117"/>
+      <c r="AU5" s="114"/>
+      <c r="AV5" s="115"/>
+      <c r="AW5" s="116"/>
+      <c r="AX5" s="116"/>
+      <c r="AY5" s="116"/>
+      <c r="AZ5" s="117"/>
+      <c r="BA5" s="114"/>
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="116"/>
+      <c r="BD5" s="116"/>
+      <c r="BE5" s="116"/>
+      <c r="BF5" s="118"/>
+      <c r="BG5" s="114"/>
+      <c r="BH5" s="115"/>
+      <c r="BI5" s="116"/>
+      <c r="BJ5" s="116"/>
+      <c r="BK5" s="116"/>
+      <c r="BL5" s="117"/>
+      <c r="BM5" s="114"/>
+      <c r="BN5" s="115"/>
+      <c r="BO5" s="116"/>
+      <c r="BP5" s="116"/>
+      <c r="BQ5" s="116"/>
+      <c r="BR5" s="117"/>
+      <c r="BS5" s="114"/>
+      <c r="BT5" s="115"/>
+      <c r="BU5" s="116"/>
+      <c r="BV5" s="116"/>
+      <c r="BW5" s="116"/>
+      <c r="BX5" s="117"/>
     </row>
     <row r="6" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="105"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="111" t="s">
+      <c r="A6" s="156"/>
+      <c r="B6" s="167"/>
+      <c r="C6" s="160" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="45">
@@ -4140,59 +4140,59 @@
       <c r="AB6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AC6" s="147"/>
-      <c r="AD6" s="148"/>
-      <c r="AE6" s="149"/>
-      <c r="AF6" s="149"/>
-      <c r="AG6" s="149"/>
-      <c r="AH6" s="150"/>
-      <c r="AI6" s="147"/>
-      <c r="AJ6" s="148"/>
-      <c r="AK6" s="149"/>
-      <c r="AL6" s="149"/>
-      <c r="AM6" s="149"/>
-      <c r="AN6" s="150"/>
-      <c r="AO6" s="148"/>
-      <c r="AP6" s="148"/>
-      <c r="AQ6" s="149"/>
-      <c r="AR6" s="149"/>
-      <c r="AS6" s="149"/>
-      <c r="AT6" s="150"/>
-      <c r="AU6" s="147"/>
-      <c r="AV6" s="148"/>
-      <c r="AW6" s="149"/>
-      <c r="AX6" s="149"/>
-      <c r="AY6" s="149"/>
-      <c r="AZ6" s="150"/>
-      <c r="BA6" s="147"/>
-      <c r="BB6" s="148"/>
-      <c r="BC6" s="149"/>
-      <c r="BD6" s="149"/>
-      <c r="BE6" s="149"/>
-      <c r="BF6" s="151"/>
-      <c r="BG6" s="147"/>
-      <c r="BH6" s="148"/>
-      <c r="BI6" s="149"/>
-      <c r="BJ6" s="149"/>
-      <c r="BK6" s="149"/>
-      <c r="BL6" s="150"/>
-      <c r="BM6" s="147"/>
-      <c r="BN6" s="148"/>
-      <c r="BO6" s="149"/>
-      <c r="BP6" s="149"/>
-      <c r="BQ6" s="149"/>
-      <c r="BR6" s="150"/>
-      <c r="BS6" s="147"/>
-      <c r="BT6" s="148"/>
-      <c r="BU6" s="149"/>
-      <c r="BV6" s="149"/>
-      <c r="BW6" s="149"/>
-      <c r="BX6" s="150"/>
+      <c r="AC6" s="119"/>
+      <c r="AD6" s="120"/>
+      <c r="AE6" s="121"/>
+      <c r="AF6" s="121"/>
+      <c r="AG6" s="121"/>
+      <c r="AH6" s="122"/>
+      <c r="AI6" s="119"/>
+      <c r="AJ6" s="120"/>
+      <c r="AK6" s="121"/>
+      <c r="AL6" s="121"/>
+      <c r="AM6" s="121"/>
+      <c r="AN6" s="122"/>
+      <c r="AO6" s="120"/>
+      <c r="AP6" s="120"/>
+      <c r="AQ6" s="121"/>
+      <c r="AR6" s="121"/>
+      <c r="AS6" s="121"/>
+      <c r="AT6" s="122"/>
+      <c r="AU6" s="119"/>
+      <c r="AV6" s="120"/>
+      <c r="AW6" s="121"/>
+      <c r="AX6" s="121"/>
+      <c r="AY6" s="121"/>
+      <c r="AZ6" s="122"/>
+      <c r="BA6" s="119"/>
+      <c r="BB6" s="120"/>
+      <c r="BC6" s="121"/>
+      <c r="BD6" s="121"/>
+      <c r="BE6" s="121"/>
+      <c r="BF6" s="123"/>
+      <c r="BG6" s="119"/>
+      <c r="BH6" s="120"/>
+      <c r="BI6" s="121"/>
+      <c r="BJ6" s="121"/>
+      <c r="BK6" s="121"/>
+      <c r="BL6" s="122"/>
+      <c r="BM6" s="119"/>
+      <c r="BN6" s="120"/>
+      <c r="BO6" s="121"/>
+      <c r="BP6" s="121"/>
+      <c r="BQ6" s="121"/>
+      <c r="BR6" s="122"/>
+      <c r="BS6" s="119"/>
+      <c r="BT6" s="120"/>
+      <c r="BU6" s="121"/>
+      <c r="BV6" s="121"/>
+      <c r="BW6" s="121"/>
+      <c r="BX6" s="122"/>
     </row>
     <row r="7" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="105"/>
-      <c r="B7" s="106"/>
-      <c r="C7" s="111"/>
+      <c r="A7" s="156"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="160"/>
       <c r="D7" s="46">
         <v>2</v>
       </c>
@@ -4268,59 +4268,59 @@
       <c r="AB7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AC7" s="152"/>
-      <c r="AD7" s="153"/>
-      <c r="AE7" s="154"/>
-      <c r="AF7" s="154"/>
-      <c r="AG7" s="154"/>
-      <c r="AH7" s="155"/>
-      <c r="AI7" s="152"/>
-      <c r="AJ7" s="153"/>
-      <c r="AK7" s="154"/>
-      <c r="AL7" s="154"/>
-      <c r="AM7" s="154"/>
-      <c r="AN7" s="155"/>
-      <c r="AO7" s="153"/>
-      <c r="AP7" s="153"/>
-      <c r="AQ7" s="154"/>
-      <c r="AR7" s="154"/>
-      <c r="AS7" s="154"/>
-      <c r="AT7" s="155"/>
-      <c r="AU7" s="152"/>
-      <c r="AV7" s="153"/>
-      <c r="AW7" s="154"/>
-      <c r="AX7" s="154"/>
-      <c r="AY7" s="154"/>
-      <c r="AZ7" s="155"/>
-      <c r="BA7" s="152"/>
-      <c r="BB7" s="153"/>
-      <c r="BC7" s="154"/>
-      <c r="BD7" s="154"/>
-      <c r="BE7" s="154"/>
-      <c r="BF7" s="156"/>
-      <c r="BG7" s="152"/>
-      <c r="BH7" s="153"/>
-      <c r="BI7" s="154"/>
-      <c r="BJ7" s="154"/>
-      <c r="BK7" s="154"/>
-      <c r="BL7" s="155"/>
-      <c r="BM7" s="152"/>
-      <c r="BN7" s="153"/>
-      <c r="BO7" s="154"/>
-      <c r="BP7" s="154"/>
-      <c r="BQ7" s="154"/>
-      <c r="BR7" s="155"/>
-      <c r="BS7" s="152"/>
-      <c r="BT7" s="153"/>
-      <c r="BU7" s="154"/>
-      <c r="BV7" s="154"/>
-      <c r="BW7" s="154"/>
-      <c r="BX7" s="155"/>
+      <c r="AC7" s="124"/>
+      <c r="AD7" s="125"/>
+      <c r="AE7" s="126"/>
+      <c r="AF7" s="126"/>
+      <c r="AG7" s="126"/>
+      <c r="AH7" s="127"/>
+      <c r="AI7" s="124"/>
+      <c r="AJ7" s="125"/>
+      <c r="AK7" s="126"/>
+      <c r="AL7" s="126"/>
+      <c r="AM7" s="126"/>
+      <c r="AN7" s="127"/>
+      <c r="AO7" s="125"/>
+      <c r="AP7" s="125"/>
+      <c r="AQ7" s="126"/>
+      <c r="AR7" s="126"/>
+      <c r="AS7" s="126"/>
+      <c r="AT7" s="127"/>
+      <c r="AU7" s="124"/>
+      <c r="AV7" s="125"/>
+      <c r="AW7" s="126"/>
+      <c r="AX7" s="126"/>
+      <c r="AY7" s="126"/>
+      <c r="AZ7" s="127"/>
+      <c r="BA7" s="124"/>
+      <c r="BB7" s="125"/>
+      <c r="BC7" s="126"/>
+      <c r="BD7" s="126"/>
+      <c r="BE7" s="126"/>
+      <c r="BF7" s="128"/>
+      <c r="BG7" s="124"/>
+      <c r="BH7" s="125"/>
+      <c r="BI7" s="126"/>
+      <c r="BJ7" s="126"/>
+      <c r="BK7" s="126"/>
+      <c r="BL7" s="127"/>
+      <c r="BM7" s="124"/>
+      <c r="BN7" s="125"/>
+      <c r="BO7" s="126"/>
+      <c r="BP7" s="126"/>
+      <c r="BQ7" s="126"/>
+      <c r="BR7" s="127"/>
+      <c r="BS7" s="124"/>
+      <c r="BT7" s="125"/>
+      <c r="BU7" s="126"/>
+      <c r="BV7" s="126"/>
+      <c r="BW7" s="126"/>
+      <c r="BX7" s="127"/>
     </row>
     <row r="8" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="105"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="112"/>
+      <c r="A8" s="156"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="164"/>
       <c r="D8" s="46">
         <v>3</v>
       </c>
@@ -4396,57 +4396,57 @@
       <c r="AB8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AC8" s="152"/>
-      <c r="AD8" s="153"/>
-      <c r="AE8" s="154"/>
-      <c r="AF8" s="154"/>
-      <c r="AG8" s="154"/>
-      <c r="AH8" s="155"/>
-      <c r="AI8" s="152"/>
-      <c r="AJ8" s="153"/>
-      <c r="AK8" s="154"/>
-      <c r="AL8" s="154"/>
-      <c r="AM8" s="154"/>
-      <c r="AN8" s="155"/>
-      <c r="AO8" s="153"/>
-      <c r="AP8" s="153"/>
-      <c r="AQ8" s="154"/>
-      <c r="AR8" s="154"/>
-      <c r="AS8" s="154"/>
-      <c r="AT8" s="155"/>
-      <c r="AU8" s="152"/>
-      <c r="AV8" s="153"/>
-      <c r="AW8" s="154"/>
-      <c r="AX8" s="154"/>
-      <c r="AY8" s="154"/>
-      <c r="AZ8" s="155"/>
-      <c r="BA8" s="152"/>
-      <c r="BB8" s="153"/>
-      <c r="BC8" s="154"/>
-      <c r="BD8" s="154"/>
-      <c r="BE8" s="154"/>
-      <c r="BF8" s="156"/>
-      <c r="BG8" s="152"/>
-      <c r="BH8" s="153"/>
-      <c r="BI8" s="154"/>
-      <c r="BJ8" s="154"/>
-      <c r="BK8" s="154"/>
-      <c r="BL8" s="155"/>
-      <c r="BM8" s="152"/>
-      <c r="BN8" s="153"/>
-      <c r="BO8" s="154"/>
-      <c r="BP8" s="154"/>
-      <c r="BQ8" s="154"/>
-      <c r="BR8" s="155"/>
-      <c r="BS8" s="152"/>
-      <c r="BT8" s="153"/>
-      <c r="BU8" s="154"/>
-      <c r="BV8" s="154"/>
-      <c r="BW8" s="154"/>
-      <c r="BX8" s="155"/>
+      <c r="AC8" s="124"/>
+      <c r="AD8" s="125"/>
+      <c r="AE8" s="126"/>
+      <c r="AF8" s="126"/>
+      <c r="AG8" s="126"/>
+      <c r="AH8" s="127"/>
+      <c r="AI8" s="124"/>
+      <c r="AJ8" s="125"/>
+      <c r="AK8" s="126"/>
+      <c r="AL8" s="126"/>
+      <c r="AM8" s="126"/>
+      <c r="AN8" s="127"/>
+      <c r="AO8" s="125"/>
+      <c r="AP8" s="125"/>
+      <c r="AQ8" s="126"/>
+      <c r="AR8" s="126"/>
+      <c r="AS8" s="126"/>
+      <c r="AT8" s="127"/>
+      <c r="AU8" s="124"/>
+      <c r="AV8" s="125"/>
+      <c r="AW8" s="126"/>
+      <c r="AX8" s="126"/>
+      <c r="AY8" s="126"/>
+      <c r="AZ8" s="127"/>
+      <c r="BA8" s="124"/>
+      <c r="BB8" s="125"/>
+      <c r="BC8" s="126"/>
+      <c r="BD8" s="126"/>
+      <c r="BE8" s="126"/>
+      <c r="BF8" s="128"/>
+      <c r="BG8" s="124"/>
+      <c r="BH8" s="125"/>
+      <c r="BI8" s="126"/>
+      <c r="BJ8" s="126"/>
+      <c r="BK8" s="126"/>
+      <c r="BL8" s="127"/>
+      <c r="BM8" s="124"/>
+      <c r="BN8" s="125"/>
+      <c r="BO8" s="126"/>
+      <c r="BP8" s="126"/>
+      <c r="BQ8" s="126"/>
+      <c r="BR8" s="127"/>
+      <c r="BS8" s="124"/>
+      <c r="BT8" s="125"/>
+      <c r="BU8" s="126"/>
+      <c r="BV8" s="126"/>
+      <c r="BW8" s="126"/>
+      <c r="BX8" s="127"/>
     </row>
     <row r="9" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="105"/>
+      <c r="A9" s="156"/>
       <c r="B9" s="9"/>
       <c r="C9" s="7"/>
       <c r="D9" s="47"/>
@@ -4524,11 +4524,11 @@
       <c r="BX9" s="31"/>
     </row>
     <row r="10" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="105"/>
-      <c r="B10" s="106" t="s">
+      <c r="A10" s="156"/>
+      <c r="B10" s="167" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="157" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="46">
@@ -4606,59 +4606,59 @@
       <c r="AB10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AC10" s="157"/>
-      <c r="AD10" s="158"/>
-      <c r="AE10" s="159"/>
-      <c r="AF10" s="159"/>
-      <c r="AG10" s="159"/>
-      <c r="AH10" s="160"/>
-      <c r="AI10" s="157"/>
-      <c r="AJ10" s="158"/>
-      <c r="AK10" s="159"/>
-      <c r="AL10" s="159"/>
-      <c r="AM10" s="159"/>
-      <c r="AN10" s="160"/>
-      <c r="AO10" s="158"/>
-      <c r="AP10" s="159"/>
-      <c r="AQ10" s="159"/>
-      <c r="AR10" s="159"/>
-      <c r="AS10" s="159"/>
-      <c r="AT10" s="160"/>
-      <c r="AU10" s="157"/>
-      <c r="AV10" s="158"/>
-      <c r="AW10" s="159"/>
-      <c r="AX10" s="159"/>
-      <c r="AY10" s="159"/>
-      <c r="AZ10" s="160"/>
-      <c r="BA10" s="157"/>
-      <c r="BB10" s="158"/>
-      <c r="BC10" s="159"/>
-      <c r="BD10" s="159"/>
-      <c r="BE10" s="159"/>
-      <c r="BF10" s="161"/>
-      <c r="BG10" s="157"/>
-      <c r="BH10" s="158"/>
-      <c r="BI10" s="159"/>
-      <c r="BJ10" s="159"/>
-      <c r="BK10" s="159"/>
-      <c r="BL10" s="160"/>
-      <c r="BM10" s="157"/>
-      <c r="BN10" s="158"/>
-      <c r="BO10" s="159"/>
-      <c r="BP10" s="159"/>
-      <c r="BQ10" s="159"/>
-      <c r="BR10" s="160"/>
-      <c r="BS10" s="157"/>
-      <c r="BT10" s="158"/>
-      <c r="BU10" s="159"/>
-      <c r="BV10" s="159"/>
-      <c r="BW10" s="159"/>
-      <c r="BX10" s="160"/>
+      <c r="AC10" s="129"/>
+      <c r="AD10" s="130"/>
+      <c r="AE10" s="131"/>
+      <c r="AF10" s="131"/>
+      <c r="AG10" s="131"/>
+      <c r="AH10" s="132"/>
+      <c r="AI10" s="129"/>
+      <c r="AJ10" s="130"/>
+      <c r="AK10" s="131"/>
+      <c r="AL10" s="131"/>
+      <c r="AM10" s="131"/>
+      <c r="AN10" s="132"/>
+      <c r="AO10" s="130"/>
+      <c r="AP10" s="131"/>
+      <c r="AQ10" s="131"/>
+      <c r="AR10" s="131"/>
+      <c r="AS10" s="131"/>
+      <c r="AT10" s="132"/>
+      <c r="AU10" s="129"/>
+      <c r="AV10" s="130"/>
+      <c r="AW10" s="131"/>
+      <c r="AX10" s="131"/>
+      <c r="AY10" s="131"/>
+      <c r="AZ10" s="132"/>
+      <c r="BA10" s="129"/>
+      <c r="BB10" s="130"/>
+      <c r="BC10" s="131"/>
+      <c r="BD10" s="131"/>
+      <c r="BE10" s="131"/>
+      <c r="BF10" s="133"/>
+      <c r="BG10" s="129"/>
+      <c r="BH10" s="130"/>
+      <c r="BI10" s="131"/>
+      <c r="BJ10" s="131"/>
+      <c r="BK10" s="131"/>
+      <c r="BL10" s="132"/>
+      <c r="BM10" s="129"/>
+      <c r="BN10" s="130"/>
+      <c r="BO10" s="131"/>
+      <c r="BP10" s="131"/>
+      <c r="BQ10" s="131"/>
+      <c r="BR10" s="132"/>
+      <c r="BS10" s="129"/>
+      <c r="BT10" s="130"/>
+      <c r="BU10" s="131"/>
+      <c r="BV10" s="131"/>
+      <c r="BW10" s="131"/>
+      <c r="BX10" s="132"/>
     </row>
     <row r="11" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="105"/>
-      <c r="B11" s="106"/>
-      <c r="C11" s="109"/>
+      <c r="A11" s="156"/>
+      <c r="B11" s="167"/>
+      <c r="C11" s="158"/>
       <c r="D11" s="46">
         <v>2</v>
       </c>
@@ -4734,59 +4734,59 @@
       <c r="AB11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AC11" s="157"/>
-      <c r="AD11" s="158"/>
-      <c r="AE11" s="159"/>
-      <c r="AF11" s="159"/>
-      <c r="AG11" s="159"/>
-      <c r="AH11" s="160"/>
-      <c r="AI11" s="157"/>
-      <c r="AJ11" s="158"/>
-      <c r="AK11" s="159"/>
-      <c r="AL11" s="159"/>
-      <c r="AM11" s="159"/>
-      <c r="AN11" s="160"/>
-      <c r="AO11" s="158"/>
-      <c r="AP11" s="159"/>
-      <c r="AQ11" s="159"/>
-      <c r="AR11" s="159"/>
-      <c r="AS11" s="159"/>
-      <c r="AT11" s="160"/>
-      <c r="AU11" s="157"/>
-      <c r="AV11" s="158"/>
-      <c r="AW11" s="159"/>
-      <c r="AX11" s="159"/>
-      <c r="AY11" s="159"/>
-      <c r="AZ11" s="160"/>
-      <c r="BA11" s="157"/>
-      <c r="BB11" s="158"/>
-      <c r="BC11" s="159"/>
-      <c r="BD11" s="159"/>
-      <c r="BE11" s="159"/>
-      <c r="BF11" s="161"/>
-      <c r="BG11" s="157"/>
-      <c r="BH11" s="158"/>
-      <c r="BI11" s="159"/>
-      <c r="BJ11" s="159"/>
-      <c r="BK11" s="159"/>
-      <c r="BL11" s="160"/>
-      <c r="BM11" s="157"/>
-      <c r="BN11" s="158"/>
-      <c r="BO11" s="159"/>
-      <c r="BP11" s="159"/>
-      <c r="BQ11" s="159"/>
-      <c r="BR11" s="160"/>
-      <c r="BS11" s="157"/>
-      <c r="BT11" s="158"/>
-      <c r="BU11" s="159"/>
-      <c r="BV11" s="159"/>
-      <c r="BW11" s="159"/>
-      <c r="BX11" s="160"/>
+      <c r="AC11" s="129"/>
+      <c r="AD11" s="130"/>
+      <c r="AE11" s="131"/>
+      <c r="AF11" s="131"/>
+      <c r="AG11" s="131"/>
+      <c r="AH11" s="132"/>
+      <c r="AI11" s="129"/>
+      <c r="AJ11" s="130"/>
+      <c r="AK11" s="131"/>
+      <c r="AL11" s="131"/>
+      <c r="AM11" s="131"/>
+      <c r="AN11" s="132"/>
+      <c r="AO11" s="130"/>
+      <c r="AP11" s="131"/>
+      <c r="AQ11" s="131"/>
+      <c r="AR11" s="131"/>
+      <c r="AS11" s="131"/>
+      <c r="AT11" s="132"/>
+      <c r="AU11" s="129"/>
+      <c r="AV11" s="130"/>
+      <c r="AW11" s="131"/>
+      <c r="AX11" s="131"/>
+      <c r="AY11" s="131"/>
+      <c r="AZ11" s="132"/>
+      <c r="BA11" s="129"/>
+      <c r="BB11" s="130"/>
+      <c r="BC11" s="131"/>
+      <c r="BD11" s="131"/>
+      <c r="BE11" s="131"/>
+      <c r="BF11" s="133"/>
+      <c r="BG11" s="129"/>
+      <c r="BH11" s="130"/>
+      <c r="BI11" s="131"/>
+      <c r="BJ11" s="131"/>
+      <c r="BK11" s="131"/>
+      <c r="BL11" s="132"/>
+      <c r="BM11" s="129"/>
+      <c r="BN11" s="130"/>
+      <c r="BO11" s="131"/>
+      <c r="BP11" s="131"/>
+      <c r="BQ11" s="131"/>
+      <c r="BR11" s="132"/>
+      <c r="BS11" s="129"/>
+      <c r="BT11" s="130"/>
+      <c r="BU11" s="131"/>
+      <c r="BV11" s="131"/>
+      <c r="BW11" s="131"/>
+      <c r="BX11" s="132"/>
     </row>
     <row r="12" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="105"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="110"/>
+      <c r="A12" s="156"/>
+      <c r="B12" s="167"/>
+      <c r="C12" s="159"/>
       <c r="D12" s="100">
         <v>3</v>
       </c>
@@ -4862,296 +4862,296 @@
       <c r="AB12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AC12" s="162"/>
-      <c r="AD12" s="163"/>
-      <c r="AE12" s="164"/>
-      <c r="AF12" s="164"/>
-      <c r="AG12" s="164"/>
-      <c r="AH12" s="165"/>
-      <c r="AI12" s="162"/>
-      <c r="AJ12" s="163"/>
-      <c r="AK12" s="164"/>
-      <c r="AL12" s="164"/>
-      <c r="AM12" s="164"/>
-      <c r="AN12" s="165"/>
-      <c r="AO12" s="163"/>
-      <c r="AP12" s="164"/>
-      <c r="AQ12" s="164"/>
-      <c r="AR12" s="164"/>
-      <c r="AS12" s="164"/>
-      <c r="AT12" s="165"/>
-      <c r="AU12" s="162"/>
-      <c r="AV12" s="163"/>
-      <c r="AW12" s="164"/>
-      <c r="AX12" s="164"/>
-      <c r="AY12" s="164"/>
-      <c r="AZ12" s="165"/>
-      <c r="BA12" s="162"/>
-      <c r="BB12" s="163"/>
-      <c r="BC12" s="164"/>
-      <c r="BD12" s="164"/>
-      <c r="BE12" s="164"/>
-      <c r="BF12" s="166"/>
-      <c r="BG12" s="162"/>
-      <c r="BH12" s="163"/>
-      <c r="BI12" s="164"/>
-      <c r="BJ12" s="164"/>
-      <c r="BK12" s="164"/>
-      <c r="BL12" s="165"/>
-      <c r="BM12" s="162"/>
-      <c r="BN12" s="163"/>
-      <c r="BO12" s="164"/>
-      <c r="BP12" s="164"/>
-      <c r="BQ12" s="164"/>
-      <c r="BR12" s="165"/>
-      <c r="BS12" s="162"/>
-      <c r="BT12" s="163"/>
-      <c r="BU12" s="164"/>
-      <c r="BV12" s="164"/>
-      <c r="BW12" s="164"/>
-      <c r="BX12" s="165"/>
+      <c r="AC12" s="134"/>
+      <c r="AD12" s="135"/>
+      <c r="AE12" s="136"/>
+      <c r="AF12" s="136"/>
+      <c r="AG12" s="136"/>
+      <c r="AH12" s="137"/>
+      <c r="AI12" s="134"/>
+      <c r="AJ12" s="135"/>
+      <c r="AK12" s="136"/>
+      <c r="AL12" s="136"/>
+      <c r="AM12" s="136"/>
+      <c r="AN12" s="137"/>
+      <c r="AO12" s="135"/>
+      <c r="AP12" s="136"/>
+      <c r="AQ12" s="136"/>
+      <c r="AR12" s="136"/>
+      <c r="AS12" s="136"/>
+      <c r="AT12" s="137"/>
+      <c r="AU12" s="134"/>
+      <c r="AV12" s="135"/>
+      <c r="AW12" s="136"/>
+      <c r="AX12" s="136"/>
+      <c r="AY12" s="136"/>
+      <c r="AZ12" s="137"/>
+      <c r="BA12" s="134"/>
+      <c r="BB12" s="135"/>
+      <c r="BC12" s="136"/>
+      <c r="BD12" s="136"/>
+      <c r="BE12" s="136"/>
+      <c r="BF12" s="138"/>
+      <c r="BG12" s="134"/>
+      <c r="BH12" s="135"/>
+      <c r="BI12" s="136"/>
+      <c r="BJ12" s="136"/>
+      <c r="BK12" s="136"/>
+      <c r="BL12" s="137"/>
+      <c r="BM12" s="134"/>
+      <c r="BN12" s="135"/>
+      <c r="BO12" s="136"/>
+      <c r="BP12" s="136"/>
+      <c r="BQ12" s="136"/>
+      <c r="BR12" s="137"/>
+      <c r="BS12" s="134"/>
+      <c r="BT12" s="135"/>
+      <c r="BU12" s="136"/>
+      <c r="BV12" s="136"/>
+      <c r="BW12" s="136"/>
+      <c r="BX12" s="137"/>
     </row>
     <row r="13" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="105"/>
-      <c r="B13" s="106"/>
-      <c r="C13" s="111" t="s">
+      <c r="A13" s="156"/>
+      <c r="B13" s="167"/>
+      <c r="C13" s="160" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="45">
         <v>1</v>
       </c>
-      <c r="E13" s="148"/>
-      <c r="F13" s="149"/>
-      <c r="G13" s="149"/>
-      <c r="H13" s="149"/>
-      <c r="I13" s="149"/>
-      <c r="J13" s="150"/>
-      <c r="K13" s="147"/>
-      <c r="L13" s="148"/>
-      <c r="M13" s="149"/>
-      <c r="N13" s="149"/>
-      <c r="O13" s="149"/>
-      <c r="P13" s="150"/>
-      <c r="Q13" s="147"/>
-      <c r="R13" s="148"/>
-      <c r="S13" s="149"/>
-      <c r="T13" s="149"/>
-      <c r="U13" s="149"/>
-      <c r="V13" s="167"/>
-      <c r="W13" s="147"/>
-      <c r="X13" s="148"/>
-      <c r="Y13" s="149"/>
-      <c r="Z13" s="149"/>
-      <c r="AA13" s="149"/>
-      <c r="AB13" s="150"/>
-      <c r="AC13" s="147"/>
-      <c r="AD13" s="148"/>
-      <c r="AE13" s="149"/>
-      <c r="AF13" s="149"/>
-      <c r="AG13" s="149"/>
-      <c r="AH13" s="150"/>
-      <c r="AI13" s="147"/>
-      <c r="AJ13" s="148"/>
-      <c r="AK13" s="149"/>
-      <c r="AL13" s="149"/>
-      <c r="AM13" s="149"/>
-      <c r="AN13" s="150"/>
-      <c r="AO13" s="148"/>
-      <c r="AP13" s="149"/>
-      <c r="AQ13" s="149"/>
-      <c r="AR13" s="149"/>
-      <c r="AS13" s="149"/>
-      <c r="AT13" s="150"/>
-      <c r="AU13" s="147"/>
-      <c r="AV13" s="148"/>
-      <c r="AW13" s="149"/>
-      <c r="AX13" s="149"/>
-      <c r="AY13" s="149"/>
-      <c r="AZ13" s="150"/>
-      <c r="BA13" s="147"/>
-      <c r="BB13" s="148"/>
-      <c r="BC13" s="149"/>
-      <c r="BD13" s="149"/>
-      <c r="BE13" s="149"/>
-      <c r="BF13" s="167"/>
-      <c r="BG13" s="147"/>
-      <c r="BH13" s="148"/>
-      <c r="BI13" s="149"/>
-      <c r="BJ13" s="149"/>
-      <c r="BK13" s="149"/>
-      <c r="BL13" s="150"/>
-      <c r="BM13" s="147"/>
-      <c r="BN13" s="148"/>
-      <c r="BO13" s="149"/>
-      <c r="BP13" s="149"/>
-      <c r="BQ13" s="149"/>
-      <c r="BR13" s="150"/>
-      <c r="BS13" s="147"/>
-      <c r="BT13" s="148"/>
-      <c r="BU13" s="149"/>
-      <c r="BV13" s="149"/>
-      <c r="BW13" s="149"/>
-      <c r="BX13" s="150"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="119"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="122"/>
+      <c r="Q13" s="119"/>
+      <c r="R13" s="120"/>
+      <c r="S13" s="121"/>
+      <c r="T13" s="121"/>
+      <c r="U13" s="121"/>
+      <c r="V13" s="139"/>
+      <c r="W13" s="119"/>
+      <c r="X13" s="120"/>
+      <c r="Y13" s="121"/>
+      <c r="Z13" s="121"/>
+      <c r="AA13" s="121"/>
+      <c r="AB13" s="122"/>
+      <c r="AC13" s="119"/>
+      <c r="AD13" s="120"/>
+      <c r="AE13" s="121"/>
+      <c r="AF13" s="121"/>
+      <c r="AG13" s="121"/>
+      <c r="AH13" s="122"/>
+      <c r="AI13" s="119"/>
+      <c r="AJ13" s="120"/>
+      <c r="AK13" s="121"/>
+      <c r="AL13" s="121"/>
+      <c r="AM13" s="121"/>
+      <c r="AN13" s="122"/>
+      <c r="AO13" s="120"/>
+      <c r="AP13" s="121"/>
+      <c r="AQ13" s="121"/>
+      <c r="AR13" s="121"/>
+      <c r="AS13" s="121"/>
+      <c r="AT13" s="122"/>
+      <c r="AU13" s="119"/>
+      <c r="AV13" s="120"/>
+      <c r="AW13" s="121"/>
+      <c r="AX13" s="121"/>
+      <c r="AY13" s="121"/>
+      <c r="AZ13" s="122"/>
+      <c r="BA13" s="119"/>
+      <c r="BB13" s="120"/>
+      <c r="BC13" s="121"/>
+      <c r="BD13" s="121"/>
+      <c r="BE13" s="121"/>
+      <c r="BF13" s="139"/>
+      <c r="BG13" s="119"/>
+      <c r="BH13" s="120"/>
+      <c r="BI13" s="121"/>
+      <c r="BJ13" s="121"/>
+      <c r="BK13" s="121"/>
+      <c r="BL13" s="122"/>
+      <c r="BM13" s="119"/>
+      <c r="BN13" s="120"/>
+      <c r="BO13" s="121"/>
+      <c r="BP13" s="121"/>
+      <c r="BQ13" s="121"/>
+      <c r="BR13" s="122"/>
+      <c r="BS13" s="119"/>
+      <c r="BT13" s="120"/>
+      <c r="BU13" s="121"/>
+      <c r="BV13" s="121"/>
+      <c r="BW13" s="121"/>
+      <c r="BX13" s="122"/>
     </row>
     <row r="14" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="105"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="111"/>
+      <c r="A14" s="156"/>
+      <c r="B14" s="167"/>
+      <c r="C14" s="160"/>
       <c r="D14" s="46">
         <v>2</v>
       </c>
-      <c r="E14" s="153"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="155"/>
-      <c r="K14" s="152"/>
-      <c r="L14" s="153"/>
-      <c r="M14" s="154"/>
-      <c r="N14" s="154"/>
-      <c r="O14" s="154"/>
-      <c r="P14" s="155"/>
-      <c r="Q14" s="152"/>
-      <c r="R14" s="153"/>
-      <c r="S14" s="154"/>
-      <c r="T14" s="154"/>
-      <c r="U14" s="154"/>
-      <c r="V14" s="168"/>
-      <c r="W14" s="152"/>
-      <c r="X14" s="153"/>
-      <c r="Y14" s="154"/>
-      <c r="Z14" s="154"/>
-      <c r="AA14" s="154"/>
-      <c r="AB14" s="155"/>
-      <c r="AC14" s="152"/>
-      <c r="AD14" s="153"/>
-      <c r="AE14" s="154"/>
-      <c r="AF14" s="154"/>
-      <c r="AG14" s="154"/>
-      <c r="AH14" s="155"/>
-      <c r="AI14" s="152"/>
-      <c r="AJ14" s="153"/>
-      <c r="AK14" s="154"/>
-      <c r="AL14" s="154"/>
-      <c r="AM14" s="154"/>
-      <c r="AN14" s="155"/>
-      <c r="AO14" s="153"/>
-      <c r="AP14" s="154"/>
-      <c r="AQ14" s="154"/>
-      <c r="AR14" s="154"/>
-      <c r="AS14" s="154"/>
-      <c r="AT14" s="155"/>
-      <c r="AU14" s="152"/>
-      <c r="AV14" s="153"/>
-      <c r="AW14" s="154"/>
-      <c r="AX14" s="154"/>
-      <c r="AY14" s="154"/>
-      <c r="AZ14" s="155"/>
-      <c r="BA14" s="152"/>
-      <c r="BB14" s="153"/>
-      <c r="BC14" s="154"/>
-      <c r="BD14" s="154"/>
-      <c r="BE14" s="154"/>
-      <c r="BF14" s="168"/>
-      <c r="BG14" s="152"/>
-      <c r="BH14" s="153"/>
-      <c r="BI14" s="154"/>
-      <c r="BJ14" s="154"/>
-      <c r="BK14" s="154"/>
-      <c r="BL14" s="155"/>
-      <c r="BM14" s="152"/>
-      <c r="BN14" s="153"/>
-      <c r="BO14" s="154"/>
-      <c r="BP14" s="154"/>
-      <c r="BQ14" s="154"/>
-      <c r="BR14" s="155"/>
-      <c r="BS14" s="152"/>
-      <c r="BT14" s="153"/>
-      <c r="BU14" s="154"/>
-      <c r="BV14" s="154"/>
-      <c r="BW14" s="154"/>
-      <c r="BX14" s="155"/>
+      <c r="E14" s="125"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="126"/>
+      <c r="I14" s="126"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="125"/>
+      <c r="M14" s="126"/>
+      <c r="N14" s="126"/>
+      <c r="O14" s="126"/>
+      <c r="P14" s="127"/>
+      <c r="Q14" s="124"/>
+      <c r="R14" s="125"/>
+      <c r="S14" s="126"/>
+      <c r="T14" s="126"/>
+      <c r="U14" s="126"/>
+      <c r="V14" s="140"/>
+      <c r="W14" s="124"/>
+      <c r="X14" s="125"/>
+      <c r="Y14" s="126"/>
+      <c r="Z14" s="126"/>
+      <c r="AA14" s="126"/>
+      <c r="AB14" s="127"/>
+      <c r="AC14" s="124"/>
+      <c r="AD14" s="125"/>
+      <c r="AE14" s="126"/>
+      <c r="AF14" s="126"/>
+      <c r="AG14" s="126"/>
+      <c r="AH14" s="127"/>
+      <c r="AI14" s="124"/>
+      <c r="AJ14" s="125"/>
+      <c r="AK14" s="126"/>
+      <c r="AL14" s="126"/>
+      <c r="AM14" s="126"/>
+      <c r="AN14" s="127"/>
+      <c r="AO14" s="125"/>
+      <c r="AP14" s="126"/>
+      <c r="AQ14" s="126"/>
+      <c r="AR14" s="126"/>
+      <c r="AS14" s="126"/>
+      <c r="AT14" s="127"/>
+      <c r="AU14" s="124"/>
+      <c r="AV14" s="125"/>
+      <c r="AW14" s="126"/>
+      <c r="AX14" s="126"/>
+      <c r="AY14" s="126"/>
+      <c r="AZ14" s="127"/>
+      <c r="BA14" s="124"/>
+      <c r="BB14" s="125"/>
+      <c r="BC14" s="126"/>
+      <c r="BD14" s="126"/>
+      <c r="BE14" s="126"/>
+      <c r="BF14" s="140"/>
+      <c r="BG14" s="124"/>
+      <c r="BH14" s="125"/>
+      <c r="BI14" s="126"/>
+      <c r="BJ14" s="126"/>
+      <c r="BK14" s="126"/>
+      <c r="BL14" s="127"/>
+      <c r="BM14" s="124"/>
+      <c r="BN14" s="125"/>
+      <c r="BO14" s="126"/>
+      <c r="BP14" s="126"/>
+      <c r="BQ14" s="126"/>
+      <c r="BR14" s="127"/>
+      <c r="BS14" s="124"/>
+      <c r="BT14" s="125"/>
+      <c r="BU14" s="126"/>
+      <c r="BV14" s="126"/>
+      <c r="BW14" s="126"/>
+      <c r="BX14" s="127"/>
     </row>
     <row r="15" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="105"/>
-      <c r="B15" s="106"/>
-      <c r="C15" s="112"/>
+      <c r="A15" s="156"/>
+      <c r="B15" s="167"/>
+      <c r="C15" s="164"/>
       <c r="D15" s="46">
         <v>3</v>
       </c>
-      <c r="E15" s="153"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="155"/>
-      <c r="K15" s="152"/>
-      <c r="L15" s="153"/>
-      <c r="M15" s="154"/>
-      <c r="N15" s="154"/>
-      <c r="O15" s="154"/>
-      <c r="P15" s="155"/>
-      <c r="Q15" s="152"/>
-      <c r="R15" s="153"/>
-      <c r="S15" s="154"/>
-      <c r="T15" s="154"/>
-      <c r="U15" s="154"/>
-      <c r="V15" s="168"/>
-      <c r="W15" s="152"/>
-      <c r="X15" s="153"/>
-      <c r="Y15" s="154"/>
-      <c r="Z15" s="154"/>
-      <c r="AA15" s="154"/>
-      <c r="AB15" s="155"/>
-      <c r="AC15" s="152"/>
-      <c r="AD15" s="153"/>
-      <c r="AE15" s="154"/>
-      <c r="AF15" s="154"/>
-      <c r="AG15" s="154"/>
-      <c r="AH15" s="155"/>
-      <c r="AI15" s="152"/>
-      <c r="AJ15" s="153"/>
-      <c r="AK15" s="154"/>
-      <c r="AL15" s="154"/>
-      <c r="AM15" s="154"/>
-      <c r="AN15" s="155"/>
-      <c r="AO15" s="153"/>
-      <c r="AP15" s="154"/>
-      <c r="AQ15" s="154"/>
-      <c r="AR15" s="154"/>
-      <c r="AS15" s="154"/>
-      <c r="AT15" s="155"/>
-      <c r="AU15" s="152"/>
-      <c r="AV15" s="153"/>
-      <c r="AW15" s="154"/>
-      <c r="AX15" s="154"/>
-      <c r="AY15" s="154"/>
-      <c r="AZ15" s="155"/>
-      <c r="BA15" s="152"/>
-      <c r="BB15" s="153"/>
-      <c r="BC15" s="154"/>
-      <c r="BD15" s="154"/>
-      <c r="BE15" s="154"/>
-      <c r="BF15" s="168"/>
-      <c r="BG15" s="152"/>
-      <c r="BH15" s="153"/>
-      <c r="BI15" s="154"/>
-      <c r="BJ15" s="154"/>
-      <c r="BK15" s="154"/>
-      <c r="BL15" s="155"/>
-      <c r="BM15" s="152"/>
-      <c r="BN15" s="153"/>
-      <c r="BO15" s="154"/>
-      <c r="BP15" s="154"/>
-      <c r="BQ15" s="154"/>
-      <c r="BR15" s="155"/>
-      <c r="BS15" s="152"/>
-      <c r="BT15" s="153"/>
-      <c r="BU15" s="154"/>
-      <c r="BV15" s="154"/>
-      <c r="BW15" s="154"/>
-      <c r="BX15" s="155"/>
+      <c r="E15" s="125"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="126"/>
+      <c r="H15" s="126"/>
+      <c r="I15" s="126"/>
+      <c r="J15" s="127"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="125"/>
+      <c r="M15" s="126"/>
+      <c r="N15" s="126"/>
+      <c r="O15" s="126"/>
+      <c r="P15" s="127"/>
+      <c r="Q15" s="124"/>
+      <c r="R15" s="125"/>
+      <c r="S15" s="126"/>
+      <c r="T15" s="126"/>
+      <c r="U15" s="126"/>
+      <c r="V15" s="140"/>
+      <c r="W15" s="124"/>
+      <c r="X15" s="125"/>
+      <c r="Y15" s="126"/>
+      <c r="Z15" s="126"/>
+      <c r="AA15" s="126"/>
+      <c r="AB15" s="127"/>
+      <c r="AC15" s="124"/>
+      <c r="AD15" s="125"/>
+      <c r="AE15" s="126"/>
+      <c r="AF15" s="126"/>
+      <c r="AG15" s="126"/>
+      <c r="AH15" s="127"/>
+      <c r="AI15" s="124"/>
+      <c r="AJ15" s="125"/>
+      <c r="AK15" s="126"/>
+      <c r="AL15" s="126"/>
+      <c r="AM15" s="126"/>
+      <c r="AN15" s="127"/>
+      <c r="AO15" s="125"/>
+      <c r="AP15" s="126"/>
+      <c r="AQ15" s="126"/>
+      <c r="AR15" s="126"/>
+      <c r="AS15" s="126"/>
+      <c r="AT15" s="127"/>
+      <c r="AU15" s="124"/>
+      <c r="AV15" s="125"/>
+      <c r="AW15" s="126"/>
+      <c r="AX15" s="126"/>
+      <c r="AY15" s="126"/>
+      <c r="AZ15" s="127"/>
+      <c r="BA15" s="124"/>
+      <c r="BB15" s="125"/>
+      <c r="BC15" s="126"/>
+      <c r="BD15" s="126"/>
+      <c r="BE15" s="126"/>
+      <c r="BF15" s="140"/>
+      <c r="BG15" s="124"/>
+      <c r="BH15" s="125"/>
+      <c r="BI15" s="126"/>
+      <c r="BJ15" s="126"/>
+      <c r="BK15" s="126"/>
+      <c r="BL15" s="127"/>
+      <c r="BM15" s="124"/>
+      <c r="BN15" s="125"/>
+      <c r="BO15" s="126"/>
+      <c r="BP15" s="126"/>
+      <c r="BQ15" s="126"/>
+      <c r="BR15" s="127"/>
+      <c r="BS15" s="124"/>
+      <c r="BT15" s="125"/>
+      <c r="BU15" s="126"/>
+      <c r="BV15" s="126"/>
+      <c r="BW15" s="126"/>
+      <c r="BX15" s="127"/>
     </row>
     <row r="16" spans="1:76" x14ac:dyDescent="0.5">
       <c r="A16" s="8"/>
@@ -5310,13 +5310,13 @@
       <c r="BX17" s="42"/>
     </row>
     <row r="18" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="105" t="s">
+      <c r="A18" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="167" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="114" t="s">
+      <c r="C18" s="169" t="s">
         <v>200</v>
       </c>
       <c r="D18" s="46">
@@ -5540,9 +5540,9 @@
       </c>
     </row>
     <row r="19" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="105"/>
-      <c r="B19" s="106"/>
-      <c r="C19" s="115"/>
+      <c r="A19" s="156"/>
+      <c r="B19" s="167"/>
+      <c r="C19" s="170"/>
       <c r="D19" s="46">
         <v>2</v>
       </c>
@@ -5764,9 +5764,9 @@
       </c>
     </row>
     <row r="20" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="105"/>
-      <c r="B20" s="106"/>
-      <c r="C20" s="116"/>
+      <c r="A20" s="156"/>
+      <c r="B20" s="167"/>
+      <c r="C20" s="171"/>
       <c r="D20" s="100">
         <v>3</v>
       </c>
@@ -5988,9 +5988,9 @@
       </c>
     </row>
     <row r="21" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="105"/>
-      <c r="B21" s="106"/>
-      <c r="C21" s="117" t="s">
+      <c r="A21" s="156"/>
+      <c r="B21" s="167"/>
+      <c r="C21" s="165" t="s">
         <v>201</v>
       </c>
       <c r="D21" s="45">
@@ -6214,9 +6214,9 @@
       </c>
     </row>
     <row r="22" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="105"/>
-      <c r="B22" s="106"/>
-      <c r="C22" s="117"/>
+      <c r="A22" s="156"/>
+      <c r="B22" s="167"/>
+      <c r="C22" s="165"/>
       <c r="D22" s="46">
         <v>2</v>
       </c>
@@ -6438,9 +6438,9 @@
       </c>
     </row>
     <row r="23" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="105"/>
-      <c r="B23" s="106"/>
-      <c r="C23" s="118"/>
+      <c r="A23" s="156"/>
+      <c r="B23" s="167"/>
+      <c r="C23" s="166"/>
       <c r="D23" s="46">
         <v>3</v>
       </c>
@@ -6662,7 +6662,7 @@
       </c>
     </row>
     <row r="24" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="105"/>
+      <c r="A24" s="156"/>
       <c r="B24" s="9"/>
       <c r="C24" s="7"/>
       <c r="D24" s="47"/>
@@ -6740,11 +6740,11 @@
       <c r="BX24" s="31"/>
     </row>
     <row r="25" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="105"/>
-      <c r="B25" s="106" t="s">
+      <c r="A25" s="156"/>
+      <c r="B25" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="113" t="s">
+      <c r="C25" s="157" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="46">
@@ -6930,23 +6930,23 @@
       <c r="BL25" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="BM25" s="157"/>
-      <c r="BN25" s="158"/>
-      <c r="BO25" s="159"/>
-      <c r="BP25" s="159"/>
-      <c r="BQ25" s="159"/>
-      <c r="BR25" s="160"/>
-      <c r="BS25" s="157"/>
-      <c r="BT25" s="158"/>
-      <c r="BU25" s="159"/>
-      <c r="BV25" s="159"/>
-      <c r="BW25" s="159"/>
-      <c r="BX25" s="160"/>
+      <c r="BM25" s="129"/>
+      <c r="BN25" s="130"/>
+      <c r="BO25" s="131"/>
+      <c r="BP25" s="131"/>
+      <c r="BQ25" s="131"/>
+      <c r="BR25" s="132"/>
+      <c r="BS25" s="129"/>
+      <c r="BT25" s="130"/>
+      <c r="BU25" s="131"/>
+      <c r="BV25" s="131"/>
+      <c r="BW25" s="131"/>
+      <c r="BX25" s="132"/>
     </row>
     <row r="26" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="105"/>
-      <c r="B26" s="106"/>
-      <c r="C26" s="109"/>
+      <c r="A26" s="156"/>
+      <c r="B26" s="167"/>
+      <c r="C26" s="158"/>
       <c r="D26" s="46">
         <v>2</v>
       </c>
@@ -7130,23 +7130,23 @@
       <c r="BL26" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="BM26" s="157"/>
-      <c r="BN26" s="158"/>
-      <c r="BO26" s="159"/>
-      <c r="BP26" s="159"/>
-      <c r="BQ26" s="159"/>
-      <c r="BR26" s="160"/>
-      <c r="BS26" s="157"/>
-      <c r="BT26" s="158"/>
-      <c r="BU26" s="159"/>
-      <c r="BV26" s="159"/>
-      <c r="BW26" s="159"/>
-      <c r="BX26" s="160"/>
+      <c r="BM26" s="129"/>
+      <c r="BN26" s="130"/>
+      <c r="BO26" s="131"/>
+      <c r="BP26" s="131"/>
+      <c r="BQ26" s="131"/>
+      <c r="BR26" s="132"/>
+      <c r="BS26" s="129"/>
+      <c r="BT26" s="130"/>
+      <c r="BU26" s="131"/>
+      <c r="BV26" s="131"/>
+      <c r="BW26" s="131"/>
+      <c r="BX26" s="132"/>
     </row>
     <row r="27" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="105"/>
-      <c r="B27" s="106"/>
-      <c r="C27" s="110"/>
+      <c r="A27" s="156"/>
+      <c r="B27" s="167"/>
+      <c r="C27" s="159"/>
       <c r="D27" s="100">
         <v>3</v>
       </c>
@@ -7330,260 +7330,260 @@
       <c r="BL27" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="BM27" s="162"/>
-      <c r="BN27" s="163"/>
-      <c r="BO27" s="164"/>
-      <c r="BP27" s="164"/>
-      <c r="BQ27" s="164"/>
-      <c r="BR27" s="165"/>
-      <c r="BS27" s="162"/>
-      <c r="BT27" s="163"/>
-      <c r="BU27" s="164"/>
-      <c r="BV27" s="164"/>
-      <c r="BW27" s="164"/>
-      <c r="BX27" s="165"/>
+      <c r="BM27" s="134"/>
+      <c r="BN27" s="135"/>
+      <c r="BO27" s="136"/>
+      <c r="BP27" s="136"/>
+      <c r="BQ27" s="136"/>
+      <c r="BR27" s="137"/>
+      <c r="BS27" s="134"/>
+      <c r="BT27" s="135"/>
+      <c r="BU27" s="136"/>
+      <c r="BV27" s="136"/>
+      <c r="BW27" s="136"/>
+      <c r="BX27" s="137"/>
     </row>
     <row r="28" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="105"/>
-      <c r="B28" s="106"/>
-      <c r="C28" s="111" t="s">
+      <c r="A28" s="156"/>
+      <c r="B28" s="167"/>
+      <c r="C28" s="160" t="s">
         <v>46</v>
       </c>
       <c r="D28" s="45">
         <v>1</v>
       </c>
-      <c r="E28" s="169"/>
-      <c r="F28" s="170"/>
-      <c r="G28" s="170"/>
-      <c r="H28" s="170"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="171"/>
-      <c r="K28" s="172"/>
-      <c r="L28" s="169"/>
-      <c r="M28" s="170"/>
-      <c r="N28" s="170"/>
-      <c r="O28" s="170"/>
-      <c r="P28" s="171"/>
-      <c r="Q28" s="172"/>
-      <c r="R28" s="169"/>
-      <c r="S28" s="170"/>
-      <c r="T28" s="170"/>
-      <c r="U28" s="170"/>
-      <c r="V28" s="173"/>
-      <c r="W28" s="172"/>
-      <c r="X28" s="169"/>
-      <c r="Y28" s="170"/>
-      <c r="Z28" s="170"/>
-      <c r="AA28" s="170"/>
-      <c r="AB28" s="171"/>
-      <c r="AC28" s="172"/>
-      <c r="AD28" s="169"/>
-      <c r="AE28" s="170"/>
-      <c r="AF28" s="170"/>
-      <c r="AG28" s="170"/>
-      <c r="AH28" s="171"/>
-      <c r="AI28" s="172"/>
-      <c r="AJ28" s="169"/>
-      <c r="AK28" s="170"/>
-      <c r="AL28" s="170"/>
-      <c r="AM28" s="170"/>
-      <c r="AN28" s="171"/>
-      <c r="AO28" s="169"/>
-      <c r="AP28" s="170"/>
-      <c r="AQ28" s="170"/>
-      <c r="AR28" s="170"/>
-      <c r="AS28" s="170"/>
-      <c r="AT28" s="171"/>
-      <c r="AU28" s="172"/>
-      <c r="AV28" s="169"/>
-      <c r="AW28" s="170"/>
-      <c r="AX28" s="170"/>
-      <c r="AY28" s="170"/>
-      <c r="AZ28" s="171"/>
-      <c r="BA28" s="172"/>
-      <c r="BB28" s="169"/>
-      <c r="BC28" s="170"/>
-      <c r="BD28" s="170"/>
-      <c r="BE28" s="170"/>
-      <c r="BF28" s="173"/>
-      <c r="BG28" s="172"/>
-      <c r="BH28" s="169"/>
-      <c r="BI28" s="170"/>
-      <c r="BJ28" s="170"/>
-      <c r="BK28" s="170"/>
-      <c r="BL28" s="171"/>
-      <c r="BM28" s="172"/>
-      <c r="BN28" s="169"/>
-      <c r="BO28" s="170"/>
-      <c r="BP28" s="170"/>
-      <c r="BQ28" s="170"/>
-      <c r="BR28" s="171"/>
-      <c r="BS28" s="172"/>
-      <c r="BT28" s="169"/>
-      <c r="BU28" s="170"/>
-      <c r="BV28" s="170"/>
-      <c r="BW28" s="170"/>
-      <c r="BX28" s="171"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="142"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="142"/>
+      <c r="I28" s="142"/>
+      <c r="J28" s="143"/>
+      <c r="K28" s="144"/>
+      <c r="L28" s="141"/>
+      <c r="M28" s="142"/>
+      <c r="N28" s="142"/>
+      <c r="O28" s="142"/>
+      <c r="P28" s="143"/>
+      <c r="Q28" s="144"/>
+      <c r="R28" s="141"/>
+      <c r="S28" s="142"/>
+      <c r="T28" s="142"/>
+      <c r="U28" s="142"/>
+      <c r="V28" s="145"/>
+      <c r="W28" s="144"/>
+      <c r="X28" s="141"/>
+      <c r="Y28" s="142"/>
+      <c r="Z28" s="142"/>
+      <c r="AA28" s="142"/>
+      <c r="AB28" s="143"/>
+      <c r="AC28" s="144"/>
+      <c r="AD28" s="141"/>
+      <c r="AE28" s="142"/>
+      <c r="AF28" s="142"/>
+      <c r="AG28" s="142"/>
+      <c r="AH28" s="143"/>
+      <c r="AI28" s="144"/>
+      <c r="AJ28" s="141"/>
+      <c r="AK28" s="142"/>
+      <c r="AL28" s="142"/>
+      <c r="AM28" s="142"/>
+      <c r="AN28" s="143"/>
+      <c r="AO28" s="141"/>
+      <c r="AP28" s="142"/>
+      <c r="AQ28" s="142"/>
+      <c r="AR28" s="142"/>
+      <c r="AS28" s="142"/>
+      <c r="AT28" s="143"/>
+      <c r="AU28" s="144"/>
+      <c r="AV28" s="141"/>
+      <c r="AW28" s="142"/>
+      <c r="AX28" s="142"/>
+      <c r="AY28" s="142"/>
+      <c r="AZ28" s="143"/>
+      <c r="BA28" s="144"/>
+      <c r="BB28" s="141"/>
+      <c r="BC28" s="142"/>
+      <c r="BD28" s="142"/>
+      <c r="BE28" s="142"/>
+      <c r="BF28" s="145"/>
+      <c r="BG28" s="144"/>
+      <c r="BH28" s="141"/>
+      <c r="BI28" s="142"/>
+      <c r="BJ28" s="142"/>
+      <c r="BK28" s="142"/>
+      <c r="BL28" s="143"/>
+      <c r="BM28" s="144"/>
+      <c r="BN28" s="141"/>
+      <c r="BO28" s="142"/>
+      <c r="BP28" s="142"/>
+      <c r="BQ28" s="142"/>
+      <c r="BR28" s="143"/>
+      <c r="BS28" s="144"/>
+      <c r="BT28" s="141"/>
+      <c r="BU28" s="142"/>
+      <c r="BV28" s="142"/>
+      <c r="BW28" s="142"/>
+      <c r="BX28" s="143"/>
     </row>
     <row r="29" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="105"/>
-      <c r="B29" s="106"/>
-      <c r="C29" s="111"/>
+      <c r="A29" s="156"/>
+      <c r="B29" s="167"/>
+      <c r="C29" s="160"/>
       <c r="D29" s="46">
         <v>2</v>
       </c>
-      <c r="E29" s="158"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
-      <c r="H29" s="159"/>
-      <c r="I29" s="159"/>
-      <c r="J29" s="160"/>
-      <c r="K29" s="157"/>
-      <c r="L29" s="158"/>
-      <c r="M29" s="159"/>
-      <c r="N29" s="159"/>
-      <c r="O29" s="159"/>
-      <c r="P29" s="160"/>
-      <c r="Q29" s="157"/>
-      <c r="R29" s="158"/>
-      <c r="S29" s="159"/>
-      <c r="T29" s="159"/>
-      <c r="U29" s="159"/>
-      <c r="V29" s="174"/>
-      <c r="W29" s="157"/>
-      <c r="X29" s="158"/>
-      <c r="Y29" s="159"/>
-      <c r="Z29" s="159"/>
-      <c r="AA29" s="159"/>
-      <c r="AB29" s="160"/>
-      <c r="AC29" s="157"/>
-      <c r="AD29" s="158"/>
-      <c r="AE29" s="159"/>
-      <c r="AF29" s="159"/>
-      <c r="AG29" s="159"/>
-      <c r="AH29" s="160"/>
-      <c r="AI29" s="157"/>
-      <c r="AJ29" s="158"/>
-      <c r="AK29" s="159"/>
-      <c r="AL29" s="159"/>
-      <c r="AM29" s="159"/>
-      <c r="AN29" s="160"/>
-      <c r="AO29" s="158"/>
-      <c r="AP29" s="159"/>
-      <c r="AQ29" s="159"/>
-      <c r="AR29" s="159"/>
-      <c r="AS29" s="159"/>
-      <c r="AT29" s="160"/>
-      <c r="AU29" s="157"/>
-      <c r="AV29" s="158"/>
-      <c r="AW29" s="159"/>
-      <c r="AX29" s="159"/>
-      <c r="AY29" s="159"/>
-      <c r="AZ29" s="160"/>
-      <c r="BA29" s="157"/>
-      <c r="BB29" s="158"/>
-      <c r="BC29" s="159"/>
-      <c r="BD29" s="159"/>
-      <c r="BE29" s="159"/>
-      <c r="BF29" s="174"/>
-      <c r="BG29" s="157"/>
-      <c r="BH29" s="158"/>
-      <c r="BI29" s="159"/>
-      <c r="BJ29" s="159"/>
-      <c r="BK29" s="159"/>
-      <c r="BL29" s="160"/>
-      <c r="BM29" s="157"/>
-      <c r="BN29" s="158"/>
-      <c r="BO29" s="159"/>
-      <c r="BP29" s="159"/>
-      <c r="BQ29" s="159"/>
-      <c r="BR29" s="160"/>
-      <c r="BS29" s="157"/>
-      <c r="BT29" s="158"/>
-      <c r="BU29" s="159"/>
-      <c r="BV29" s="159"/>
-      <c r="BW29" s="159"/>
-      <c r="BX29" s="160"/>
+      <c r="E29" s="130"/>
+      <c r="F29" s="131"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="131"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="132"/>
+      <c r="K29" s="129"/>
+      <c r="L29" s="130"/>
+      <c r="M29" s="131"/>
+      <c r="N29" s="131"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="132"/>
+      <c r="Q29" s="129"/>
+      <c r="R29" s="130"/>
+      <c r="S29" s="131"/>
+      <c r="T29" s="131"/>
+      <c r="U29" s="131"/>
+      <c r="V29" s="146"/>
+      <c r="W29" s="129"/>
+      <c r="X29" s="130"/>
+      <c r="Y29" s="131"/>
+      <c r="Z29" s="131"/>
+      <c r="AA29" s="131"/>
+      <c r="AB29" s="132"/>
+      <c r="AC29" s="129"/>
+      <c r="AD29" s="130"/>
+      <c r="AE29" s="131"/>
+      <c r="AF29" s="131"/>
+      <c r="AG29" s="131"/>
+      <c r="AH29" s="132"/>
+      <c r="AI29" s="129"/>
+      <c r="AJ29" s="130"/>
+      <c r="AK29" s="131"/>
+      <c r="AL29" s="131"/>
+      <c r="AM29" s="131"/>
+      <c r="AN29" s="132"/>
+      <c r="AO29" s="130"/>
+      <c r="AP29" s="131"/>
+      <c r="AQ29" s="131"/>
+      <c r="AR29" s="131"/>
+      <c r="AS29" s="131"/>
+      <c r="AT29" s="132"/>
+      <c r="AU29" s="129"/>
+      <c r="AV29" s="130"/>
+      <c r="AW29" s="131"/>
+      <c r="AX29" s="131"/>
+      <c r="AY29" s="131"/>
+      <c r="AZ29" s="132"/>
+      <c r="BA29" s="129"/>
+      <c r="BB29" s="130"/>
+      <c r="BC29" s="131"/>
+      <c r="BD29" s="131"/>
+      <c r="BE29" s="131"/>
+      <c r="BF29" s="146"/>
+      <c r="BG29" s="129"/>
+      <c r="BH29" s="130"/>
+      <c r="BI29" s="131"/>
+      <c r="BJ29" s="131"/>
+      <c r="BK29" s="131"/>
+      <c r="BL29" s="132"/>
+      <c r="BM29" s="129"/>
+      <c r="BN29" s="130"/>
+      <c r="BO29" s="131"/>
+      <c r="BP29" s="131"/>
+      <c r="BQ29" s="131"/>
+      <c r="BR29" s="132"/>
+      <c r="BS29" s="129"/>
+      <c r="BT29" s="130"/>
+      <c r="BU29" s="131"/>
+      <c r="BV29" s="131"/>
+      <c r="BW29" s="131"/>
+      <c r="BX29" s="132"/>
     </row>
     <row r="30" spans="1:76" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="105"/>
-      <c r="B30" s="106"/>
-      <c r="C30" s="112"/>
+      <c r="A30" s="156"/>
+      <c r="B30" s="167"/>
+      <c r="C30" s="164"/>
       <c r="D30" s="46">
         <v>3</v>
       </c>
-      <c r="E30" s="158"/>
-      <c r="F30" s="159"/>
-      <c r="G30" s="159"/>
-      <c r="H30" s="159"/>
-      <c r="I30" s="159"/>
-      <c r="J30" s="160"/>
-      <c r="K30" s="157"/>
-      <c r="L30" s="158"/>
-      <c r="M30" s="159"/>
-      <c r="N30" s="159"/>
-      <c r="O30" s="159"/>
-      <c r="P30" s="160"/>
-      <c r="Q30" s="157"/>
-      <c r="R30" s="158"/>
-      <c r="S30" s="159"/>
-      <c r="T30" s="159"/>
-      <c r="U30" s="159"/>
-      <c r="V30" s="174"/>
-      <c r="W30" s="157"/>
-      <c r="X30" s="158"/>
-      <c r="Y30" s="159"/>
-      <c r="Z30" s="159"/>
-      <c r="AA30" s="159"/>
-      <c r="AB30" s="160"/>
-      <c r="AC30" s="157"/>
-      <c r="AD30" s="158"/>
-      <c r="AE30" s="159"/>
-      <c r="AF30" s="159"/>
-      <c r="AG30" s="159"/>
-      <c r="AH30" s="160"/>
-      <c r="AI30" s="157"/>
-      <c r="AJ30" s="158"/>
-      <c r="AK30" s="159"/>
-      <c r="AL30" s="159"/>
-      <c r="AM30" s="159"/>
-      <c r="AN30" s="160"/>
-      <c r="AO30" s="158"/>
-      <c r="AP30" s="159"/>
-      <c r="AQ30" s="159"/>
-      <c r="AR30" s="159"/>
-      <c r="AS30" s="159"/>
-      <c r="AT30" s="160"/>
-      <c r="AU30" s="157"/>
-      <c r="AV30" s="158"/>
-      <c r="AW30" s="159"/>
-      <c r="AX30" s="159"/>
-      <c r="AY30" s="159"/>
-      <c r="AZ30" s="160"/>
-      <c r="BA30" s="157"/>
-      <c r="BB30" s="158"/>
-      <c r="BC30" s="159"/>
-      <c r="BD30" s="159"/>
-      <c r="BE30" s="159"/>
-      <c r="BF30" s="174"/>
-      <c r="BG30" s="157"/>
-      <c r="BH30" s="158"/>
-      <c r="BI30" s="159"/>
-      <c r="BJ30" s="159"/>
-      <c r="BK30" s="159"/>
-      <c r="BL30" s="160"/>
-      <c r="BM30" s="157"/>
-      <c r="BN30" s="158"/>
-      <c r="BO30" s="159"/>
-      <c r="BP30" s="159"/>
-      <c r="BQ30" s="159"/>
-      <c r="BR30" s="160"/>
-      <c r="BS30" s="157"/>
-      <c r="BT30" s="158"/>
-      <c r="BU30" s="159"/>
-      <c r="BV30" s="159"/>
-      <c r="BW30" s="159"/>
-      <c r="BX30" s="160"/>
+      <c r="E30" s="130"/>
+      <c r="F30" s="131"/>
+      <c r="G30" s="131"/>
+      <c r="H30" s="131"/>
+      <c r="I30" s="131"/>
+      <c r="J30" s="132"/>
+      <c r="K30" s="129"/>
+      <c r="L30" s="130"/>
+      <c r="M30" s="131"/>
+      <c r="N30" s="131"/>
+      <c r="O30" s="131"/>
+      <c r="P30" s="132"/>
+      <c r="Q30" s="129"/>
+      <c r="R30" s="130"/>
+      <c r="S30" s="131"/>
+      <c r="T30" s="131"/>
+      <c r="U30" s="131"/>
+      <c r="V30" s="146"/>
+      <c r="W30" s="129"/>
+      <c r="X30" s="130"/>
+      <c r="Y30" s="131"/>
+      <c r="Z30" s="131"/>
+      <c r="AA30" s="131"/>
+      <c r="AB30" s="132"/>
+      <c r="AC30" s="129"/>
+      <c r="AD30" s="130"/>
+      <c r="AE30" s="131"/>
+      <c r="AF30" s="131"/>
+      <c r="AG30" s="131"/>
+      <c r="AH30" s="132"/>
+      <c r="AI30" s="129"/>
+      <c r="AJ30" s="130"/>
+      <c r="AK30" s="131"/>
+      <c r="AL30" s="131"/>
+      <c r="AM30" s="131"/>
+      <c r="AN30" s="132"/>
+      <c r="AO30" s="130"/>
+      <c r="AP30" s="131"/>
+      <c r="AQ30" s="131"/>
+      <c r="AR30" s="131"/>
+      <c r="AS30" s="131"/>
+      <c r="AT30" s="132"/>
+      <c r="AU30" s="129"/>
+      <c r="AV30" s="130"/>
+      <c r="AW30" s="131"/>
+      <c r="AX30" s="131"/>
+      <c r="AY30" s="131"/>
+      <c r="AZ30" s="132"/>
+      <c r="BA30" s="129"/>
+      <c r="BB30" s="130"/>
+      <c r="BC30" s="131"/>
+      <c r="BD30" s="131"/>
+      <c r="BE30" s="131"/>
+      <c r="BF30" s="146"/>
+      <c r="BG30" s="129"/>
+      <c r="BH30" s="130"/>
+      <c r="BI30" s="131"/>
+      <c r="BJ30" s="131"/>
+      <c r="BK30" s="131"/>
+      <c r="BL30" s="132"/>
+      <c r="BM30" s="129"/>
+      <c r="BN30" s="130"/>
+      <c r="BO30" s="131"/>
+      <c r="BP30" s="131"/>
+      <c r="BQ30" s="131"/>
+      <c r="BR30" s="132"/>
+      <c r="BS30" s="129"/>
+      <c r="BT30" s="130"/>
+      <c r="BU30" s="131"/>
+      <c r="BV30" s="131"/>
+      <c r="BW30" s="131"/>
+      <c r="BX30" s="132"/>
     </row>
     <row r="31" spans="1:76" x14ac:dyDescent="0.5">
       <c r="A31" s="8"/>
@@ -7742,13 +7742,13 @@
       <c r="BX32" s="42"/>
     </row>
     <row r="33" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="105" t="s">
+      <c r="A33" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="167" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="113" t="s">
+      <c r="C33" s="157" t="s">
         <v>45</v>
       </c>
       <c r="D33" s="46">
@@ -7934,23 +7934,23 @@
       <c r="BL33" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="BM33" s="152"/>
-      <c r="BN33" s="153"/>
-      <c r="BO33" s="154"/>
-      <c r="BP33" s="154"/>
-      <c r="BQ33" s="154"/>
-      <c r="BR33" s="155"/>
-      <c r="BS33" s="152"/>
-      <c r="BT33" s="153"/>
-      <c r="BU33" s="154"/>
-      <c r="BV33" s="154"/>
-      <c r="BW33" s="154"/>
-      <c r="BX33" s="155"/>
+      <c r="BM33" s="124"/>
+      <c r="BN33" s="125"/>
+      <c r="BO33" s="126"/>
+      <c r="BP33" s="126"/>
+      <c r="BQ33" s="126"/>
+      <c r="BR33" s="127"/>
+      <c r="BS33" s="124"/>
+      <c r="BT33" s="125"/>
+      <c r="BU33" s="126"/>
+      <c r="BV33" s="126"/>
+      <c r="BW33" s="126"/>
+      <c r="BX33" s="127"/>
     </row>
     <row r="34" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="105"/>
-      <c r="B34" s="106"/>
-      <c r="C34" s="109"/>
+      <c r="A34" s="156"/>
+      <c r="B34" s="167"/>
+      <c r="C34" s="158"/>
       <c r="D34" s="46">
         <v>2</v>
       </c>
@@ -8134,23 +8134,23 @@
       <c r="BL34" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="BM34" s="152"/>
-      <c r="BN34" s="153"/>
-      <c r="BO34" s="154"/>
-      <c r="BP34" s="154"/>
-      <c r="BQ34" s="154"/>
-      <c r="BR34" s="155"/>
-      <c r="BS34" s="152"/>
-      <c r="BT34" s="153"/>
-      <c r="BU34" s="154"/>
-      <c r="BV34" s="154"/>
-      <c r="BW34" s="154"/>
-      <c r="BX34" s="155"/>
+      <c r="BM34" s="124"/>
+      <c r="BN34" s="125"/>
+      <c r="BO34" s="126"/>
+      <c r="BP34" s="126"/>
+      <c r="BQ34" s="126"/>
+      <c r="BR34" s="127"/>
+      <c r="BS34" s="124"/>
+      <c r="BT34" s="125"/>
+      <c r="BU34" s="126"/>
+      <c r="BV34" s="126"/>
+      <c r="BW34" s="126"/>
+      <c r="BX34" s="127"/>
     </row>
     <row r="35" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="105"/>
-      <c r="B35" s="106"/>
-      <c r="C35" s="110"/>
+      <c r="A35" s="156"/>
+      <c r="B35" s="167"/>
+      <c r="C35" s="159"/>
       <c r="D35" s="100">
         <v>3</v>
       </c>
@@ -8334,263 +8334,263 @@
       <c r="BL35" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="BM35" s="175"/>
-      <c r="BN35" s="176"/>
-      <c r="BO35" s="177"/>
-      <c r="BP35" s="177"/>
-      <c r="BQ35" s="177"/>
-      <c r="BR35" s="178"/>
-      <c r="BS35" s="175"/>
-      <c r="BT35" s="176"/>
-      <c r="BU35" s="177"/>
-      <c r="BV35" s="177"/>
-      <c r="BW35" s="177"/>
-      <c r="BX35" s="178"/>
+      <c r="BM35" s="147"/>
+      <c r="BN35" s="148"/>
+      <c r="BO35" s="149"/>
+      <c r="BP35" s="149"/>
+      <c r="BQ35" s="149"/>
+      <c r="BR35" s="150"/>
+      <c r="BS35" s="147"/>
+      <c r="BT35" s="148"/>
+      <c r="BU35" s="149"/>
+      <c r="BV35" s="149"/>
+      <c r="BW35" s="149"/>
+      <c r="BX35" s="150"/>
     </row>
     <row r="36" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="105"/>
-      <c r="B36" s="106"/>
-      <c r="C36" s="111" t="s">
+      <c r="A36" s="156"/>
+      <c r="B36" s="167"/>
+      <c r="C36" s="160" t="s">
         <v>46</v>
       </c>
       <c r="D36" s="45">
         <v>1</v>
       </c>
-      <c r="E36" s="169"/>
-      <c r="F36" s="170"/>
-      <c r="G36" s="170"/>
-      <c r="H36" s="170"/>
-      <c r="I36" s="170"/>
-      <c r="J36" s="171"/>
-      <c r="K36" s="172"/>
-      <c r="L36" s="169"/>
-      <c r="M36" s="170"/>
-      <c r="N36" s="170"/>
-      <c r="O36" s="170"/>
-      <c r="P36" s="171"/>
-      <c r="Q36" s="172"/>
-      <c r="R36" s="169"/>
-      <c r="S36" s="170"/>
-      <c r="T36" s="170"/>
-      <c r="U36" s="170"/>
-      <c r="V36" s="173"/>
-      <c r="W36" s="172"/>
-      <c r="X36" s="169"/>
-      <c r="Y36" s="170"/>
-      <c r="Z36" s="170"/>
-      <c r="AA36" s="170"/>
-      <c r="AB36" s="171"/>
-      <c r="AC36" s="172"/>
-      <c r="AD36" s="169"/>
-      <c r="AE36" s="170"/>
-      <c r="AF36" s="170"/>
-      <c r="AG36" s="170"/>
-      <c r="AH36" s="171"/>
-      <c r="AI36" s="172"/>
-      <c r="AJ36" s="169"/>
-      <c r="AK36" s="170"/>
-      <c r="AL36" s="170"/>
-      <c r="AM36" s="170"/>
-      <c r="AN36" s="171"/>
-      <c r="AO36" s="169"/>
-      <c r="AP36" s="170"/>
-      <c r="AQ36" s="170"/>
-      <c r="AR36" s="170"/>
-      <c r="AS36" s="170"/>
-      <c r="AT36" s="171"/>
-      <c r="AU36" s="172"/>
-      <c r="AV36" s="169"/>
-      <c r="AW36" s="170"/>
-      <c r="AX36" s="170"/>
-      <c r="AY36" s="170"/>
-      <c r="AZ36" s="171"/>
-      <c r="BA36" s="172"/>
-      <c r="BB36" s="169"/>
-      <c r="BC36" s="170"/>
-      <c r="BD36" s="170"/>
-      <c r="BE36" s="170"/>
-      <c r="BF36" s="173"/>
-      <c r="BG36" s="172"/>
-      <c r="BH36" s="169"/>
-      <c r="BI36" s="170"/>
-      <c r="BJ36" s="170"/>
-      <c r="BK36" s="170"/>
-      <c r="BL36" s="171"/>
-      <c r="BM36" s="172"/>
-      <c r="BN36" s="169"/>
-      <c r="BO36" s="170"/>
-      <c r="BP36" s="170"/>
-      <c r="BQ36" s="170"/>
-      <c r="BR36" s="171"/>
-      <c r="BS36" s="172"/>
-      <c r="BT36" s="169"/>
-      <c r="BU36" s="170"/>
-      <c r="BV36" s="170"/>
-      <c r="BW36" s="170"/>
-      <c r="BX36" s="171"/>
+      <c r="E36" s="141"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="142"/>
+      <c r="I36" s="142"/>
+      <c r="J36" s="143"/>
+      <c r="K36" s="144"/>
+      <c r="L36" s="141"/>
+      <c r="M36" s="142"/>
+      <c r="N36" s="142"/>
+      <c r="O36" s="142"/>
+      <c r="P36" s="143"/>
+      <c r="Q36" s="144"/>
+      <c r="R36" s="141"/>
+      <c r="S36" s="142"/>
+      <c r="T36" s="142"/>
+      <c r="U36" s="142"/>
+      <c r="V36" s="145"/>
+      <c r="W36" s="144"/>
+      <c r="X36" s="141"/>
+      <c r="Y36" s="142"/>
+      <c r="Z36" s="142"/>
+      <c r="AA36" s="142"/>
+      <c r="AB36" s="143"/>
+      <c r="AC36" s="144"/>
+      <c r="AD36" s="141"/>
+      <c r="AE36" s="142"/>
+      <c r="AF36" s="142"/>
+      <c r="AG36" s="142"/>
+      <c r="AH36" s="143"/>
+      <c r="AI36" s="144"/>
+      <c r="AJ36" s="141"/>
+      <c r="AK36" s="142"/>
+      <c r="AL36" s="142"/>
+      <c r="AM36" s="142"/>
+      <c r="AN36" s="143"/>
+      <c r="AO36" s="141"/>
+      <c r="AP36" s="142"/>
+      <c r="AQ36" s="142"/>
+      <c r="AR36" s="142"/>
+      <c r="AS36" s="142"/>
+      <c r="AT36" s="143"/>
+      <c r="AU36" s="144"/>
+      <c r="AV36" s="141"/>
+      <c r="AW36" s="142"/>
+      <c r="AX36" s="142"/>
+      <c r="AY36" s="142"/>
+      <c r="AZ36" s="143"/>
+      <c r="BA36" s="144"/>
+      <c r="BB36" s="141"/>
+      <c r="BC36" s="142"/>
+      <c r="BD36" s="142"/>
+      <c r="BE36" s="142"/>
+      <c r="BF36" s="145"/>
+      <c r="BG36" s="144"/>
+      <c r="BH36" s="141"/>
+      <c r="BI36" s="142"/>
+      <c r="BJ36" s="142"/>
+      <c r="BK36" s="142"/>
+      <c r="BL36" s="143"/>
+      <c r="BM36" s="144"/>
+      <c r="BN36" s="141"/>
+      <c r="BO36" s="142"/>
+      <c r="BP36" s="142"/>
+      <c r="BQ36" s="142"/>
+      <c r="BR36" s="143"/>
+      <c r="BS36" s="144"/>
+      <c r="BT36" s="141"/>
+      <c r="BU36" s="142"/>
+      <c r="BV36" s="142"/>
+      <c r="BW36" s="142"/>
+      <c r="BX36" s="143"/>
     </row>
     <row r="37" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="105"/>
-      <c r="B37" s="106"/>
-      <c r="C37" s="111"/>
+      <c r="A37" s="156"/>
+      <c r="B37" s="167"/>
+      <c r="C37" s="160"/>
       <c r="D37" s="46">
         <v>2</v>
       </c>
-      <c r="E37" s="158"/>
-      <c r="F37" s="159"/>
-      <c r="G37" s="159"/>
-      <c r="H37" s="159"/>
-      <c r="I37" s="159"/>
-      <c r="J37" s="160"/>
-      <c r="K37" s="157"/>
-      <c r="L37" s="158"/>
-      <c r="M37" s="159"/>
-      <c r="N37" s="159"/>
-      <c r="O37" s="159"/>
-      <c r="P37" s="160"/>
-      <c r="Q37" s="157"/>
-      <c r="R37" s="158"/>
-      <c r="S37" s="159"/>
-      <c r="T37" s="159"/>
-      <c r="U37" s="159"/>
-      <c r="V37" s="174"/>
-      <c r="W37" s="157"/>
-      <c r="X37" s="158"/>
-      <c r="Y37" s="159"/>
-      <c r="Z37" s="159"/>
-      <c r="AA37" s="159"/>
-      <c r="AB37" s="160"/>
-      <c r="AC37" s="157"/>
-      <c r="AD37" s="158"/>
-      <c r="AE37" s="159"/>
-      <c r="AF37" s="159"/>
-      <c r="AG37" s="159"/>
-      <c r="AH37" s="160"/>
-      <c r="AI37" s="157"/>
-      <c r="AJ37" s="158"/>
-      <c r="AK37" s="159"/>
-      <c r="AL37" s="159"/>
-      <c r="AM37" s="159"/>
-      <c r="AN37" s="160"/>
-      <c r="AO37" s="158"/>
-      <c r="AP37" s="159"/>
-      <c r="AQ37" s="159"/>
-      <c r="AR37" s="159"/>
-      <c r="AS37" s="159"/>
-      <c r="AT37" s="160"/>
-      <c r="AU37" s="157"/>
-      <c r="AV37" s="158"/>
-      <c r="AW37" s="159"/>
-      <c r="AX37" s="159"/>
-      <c r="AY37" s="159"/>
-      <c r="AZ37" s="160"/>
-      <c r="BA37" s="157"/>
-      <c r="BB37" s="158"/>
-      <c r="BC37" s="159"/>
-      <c r="BD37" s="159"/>
-      <c r="BE37" s="159"/>
-      <c r="BF37" s="174"/>
-      <c r="BG37" s="157"/>
-      <c r="BH37" s="158"/>
-      <c r="BI37" s="159"/>
-      <c r="BJ37" s="159"/>
-      <c r="BK37" s="159"/>
-      <c r="BL37" s="160"/>
-      <c r="BM37" s="157"/>
-      <c r="BN37" s="158"/>
-      <c r="BO37" s="159"/>
-      <c r="BP37" s="159"/>
-      <c r="BQ37" s="159"/>
-      <c r="BR37" s="160"/>
-      <c r="BS37" s="157"/>
-      <c r="BT37" s="158"/>
-      <c r="BU37" s="159"/>
-      <c r="BV37" s="159"/>
-      <c r="BW37" s="159"/>
-      <c r="BX37" s="160"/>
+      <c r="E37" s="130"/>
+      <c r="F37" s="131"/>
+      <c r="G37" s="131"/>
+      <c r="H37" s="131"/>
+      <c r="I37" s="131"/>
+      <c r="J37" s="132"/>
+      <c r="K37" s="129"/>
+      <c r="L37" s="130"/>
+      <c r="M37" s="131"/>
+      <c r="N37" s="131"/>
+      <c r="O37" s="131"/>
+      <c r="P37" s="132"/>
+      <c r="Q37" s="129"/>
+      <c r="R37" s="130"/>
+      <c r="S37" s="131"/>
+      <c r="T37" s="131"/>
+      <c r="U37" s="131"/>
+      <c r="V37" s="146"/>
+      <c r="W37" s="129"/>
+      <c r="X37" s="130"/>
+      <c r="Y37" s="131"/>
+      <c r="Z37" s="131"/>
+      <c r="AA37" s="131"/>
+      <c r="AB37" s="132"/>
+      <c r="AC37" s="129"/>
+      <c r="AD37" s="130"/>
+      <c r="AE37" s="131"/>
+      <c r="AF37" s="131"/>
+      <c r="AG37" s="131"/>
+      <c r="AH37" s="132"/>
+      <c r="AI37" s="129"/>
+      <c r="AJ37" s="130"/>
+      <c r="AK37" s="131"/>
+      <c r="AL37" s="131"/>
+      <c r="AM37" s="131"/>
+      <c r="AN37" s="132"/>
+      <c r="AO37" s="130"/>
+      <c r="AP37" s="131"/>
+      <c r="AQ37" s="131"/>
+      <c r="AR37" s="131"/>
+      <c r="AS37" s="131"/>
+      <c r="AT37" s="132"/>
+      <c r="AU37" s="129"/>
+      <c r="AV37" s="130"/>
+      <c r="AW37" s="131"/>
+      <c r="AX37" s="131"/>
+      <c r="AY37" s="131"/>
+      <c r="AZ37" s="132"/>
+      <c r="BA37" s="129"/>
+      <c r="BB37" s="130"/>
+      <c r="BC37" s="131"/>
+      <c r="BD37" s="131"/>
+      <c r="BE37" s="131"/>
+      <c r="BF37" s="146"/>
+      <c r="BG37" s="129"/>
+      <c r="BH37" s="130"/>
+      <c r="BI37" s="131"/>
+      <c r="BJ37" s="131"/>
+      <c r="BK37" s="131"/>
+      <c r="BL37" s="132"/>
+      <c r="BM37" s="129"/>
+      <c r="BN37" s="130"/>
+      <c r="BO37" s="131"/>
+      <c r="BP37" s="131"/>
+      <c r="BQ37" s="131"/>
+      <c r="BR37" s="132"/>
+      <c r="BS37" s="129"/>
+      <c r="BT37" s="130"/>
+      <c r="BU37" s="131"/>
+      <c r="BV37" s="131"/>
+      <c r="BW37" s="131"/>
+      <c r="BX37" s="132"/>
     </row>
     <row r="38" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="105"/>
-      <c r="B38" s="106"/>
-      <c r="C38" s="112"/>
+      <c r="A38" s="156"/>
+      <c r="B38" s="167"/>
+      <c r="C38" s="164"/>
       <c r="D38" s="46">
         <v>3</v>
       </c>
-      <c r="E38" s="158"/>
-      <c r="F38" s="159"/>
-      <c r="G38" s="159"/>
-      <c r="H38" s="159"/>
-      <c r="I38" s="159"/>
-      <c r="J38" s="160"/>
-      <c r="K38" s="157"/>
-      <c r="L38" s="158"/>
-      <c r="M38" s="159"/>
-      <c r="N38" s="159"/>
-      <c r="O38" s="159"/>
-      <c r="P38" s="160"/>
-      <c r="Q38" s="157"/>
-      <c r="R38" s="158"/>
-      <c r="S38" s="159"/>
-      <c r="T38" s="159"/>
-      <c r="U38" s="159"/>
-      <c r="V38" s="174"/>
-      <c r="W38" s="157"/>
-      <c r="X38" s="158"/>
-      <c r="Y38" s="159"/>
-      <c r="Z38" s="159"/>
-      <c r="AA38" s="159"/>
-      <c r="AB38" s="160"/>
-      <c r="AC38" s="157"/>
-      <c r="AD38" s="158"/>
-      <c r="AE38" s="159"/>
-      <c r="AF38" s="159"/>
-      <c r="AG38" s="159"/>
-      <c r="AH38" s="160"/>
-      <c r="AI38" s="157"/>
-      <c r="AJ38" s="158"/>
-      <c r="AK38" s="159"/>
-      <c r="AL38" s="159"/>
-      <c r="AM38" s="159"/>
-      <c r="AN38" s="160"/>
-      <c r="AO38" s="158"/>
-      <c r="AP38" s="159"/>
-      <c r="AQ38" s="159"/>
-      <c r="AR38" s="159"/>
-      <c r="AS38" s="159"/>
-      <c r="AT38" s="160"/>
-      <c r="AU38" s="157"/>
-      <c r="AV38" s="158"/>
-      <c r="AW38" s="159"/>
-      <c r="AX38" s="159"/>
-      <c r="AY38" s="159"/>
-      <c r="AZ38" s="160"/>
-      <c r="BA38" s="157"/>
-      <c r="BB38" s="158"/>
-      <c r="BC38" s="159"/>
-      <c r="BD38" s="159"/>
-      <c r="BE38" s="159"/>
-      <c r="BF38" s="174"/>
-      <c r="BG38" s="157"/>
-      <c r="BH38" s="158"/>
-      <c r="BI38" s="159"/>
-      <c r="BJ38" s="159"/>
-      <c r="BK38" s="159"/>
-      <c r="BL38" s="160"/>
-      <c r="BM38" s="157"/>
-      <c r="BN38" s="158"/>
-      <c r="BO38" s="159"/>
-      <c r="BP38" s="159"/>
-      <c r="BQ38" s="159"/>
-      <c r="BR38" s="160"/>
-      <c r="BS38" s="157"/>
-      <c r="BT38" s="158"/>
-      <c r="BU38" s="159"/>
-      <c r="BV38" s="159"/>
-      <c r="BW38" s="159"/>
-      <c r="BX38" s="160"/>
+      <c r="E38" s="130"/>
+      <c r="F38" s="131"/>
+      <c r="G38" s="131"/>
+      <c r="H38" s="131"/>
+      <c r="I38" s="131"/>
+      <c r="J38" s="132"/>
+      <c r="K38" s="129"/>
+      <c r="L38" s="130"/>
+      <c r="M38" s="131"/>
+      <c r="N38" s="131"/>
+      <c r="O38" s="131"/>
+      <c r="P38" s="132"/>
+      <c r="Q38" s="129"/>
+      <c r="R38" s="130"/>
+      <c r="S38" s="131"/>
+      <c r="T38" s="131"/>
+      <c r="U38" s="131"/>
+      <c r="V38" s="146"/>
+      <c r="W38" s="129"/>
+      <c r="X38" s="130"/>
+      <c r="Y38" s="131"/>
+      <c r="Z38" s="131"/>
+      <c r="AA38" s="131"/>
+      <c r="AB38" s="132"/>
+      <c r="AC38" s="129"/>
+      <c r="AD38" s="130"/>
+      <c r="AE38" s="131"/>
+      <c r="AF38" s="131"/>
+      <c r="AG38" s="131"/>
+      <c r="AH38" s="132"/>
+      <c r="AI38" s="129"/>
+      <c r="AJ38" s="130"/>
+      <c r="AK38" s="131"/>
+      <c r="AL38" s="131"/>
+      <c r="AM38" s="131"/>
+      <c r="AN38" s="132"/>
+      <c r="AO38" s="130"/>
+      <c r="AP38" s="131"/>
+      <c r="AQ38" s="131"/>
+      <c r="AR38" s="131"/>
+      <c r="AS38" s="131"/>
+      <c r="AT38" s="132"/>
+      <c r="AU38" s="129"/>
+      <c r="AV38" s="130"/>
+      <c r="AW38" s="131"/>
+      <c r="AX38" s="131"/>
+      <c r="AY38" s="131"/>
+      <c r="AZ38" s="132"/>
+      <c r="BA38" s="129"/>
+      <c r="BB38" s="130"/>
+      <c r="BC38" s="131"/>
+      <c r="BD38" s="131"/>
+      <c r="BE38" s="131"/>
+      <c r="BF38" s="146"/>
+      <c r="BG38" s="129"/>
+      <c r="BH38" s="130"/>
+      <c r="BI38" s="131"/>
+      <c r="BJ38" s="131"/>
+      <c r="BK38" s="131"/>
+      <c r="BL38" s="132"/>
+      <c r="BM38" s="129"/>
+      <c r="BN38" s="130"/>
+      <c r="BO38" s="131"/>
+      <c r="BP38" s="131"/>
+      <c r="BQ38" s="131"/>
+      <c r="BR38" s="132"/>
+      <c r="BS38" s="129"/>
+      <c r="BT38" s="130"/>
+      <c r="BU38" s="131"/>
+      <c r="BV38" s="131"/>
+      <c r="BW38" s="131"/>
+      <c r="BX38" s="132"/>
     </row>
     <row r="39" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="105"/>
+      <c r="A39" s="156"/>
       <c r="B39" s="9"/>
       <c r="C39" s="7"/>
       <c r="D39" s="47"/>
@@ -8668,11 +8668,11 @@
       <c r="BX39" s="31"/>
     </row>
     <row r="40" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="105"/>
-      <c r="B40" s="106" t="s">
+      <c r="A40" s="156"/>
+      <c r="B40" s="167" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="113" t="s">
+      <c r="C40" s="157" t="s">
         <v>45</v>
       </c>
       <c r="D40" s="46">
@@ -8858,23 +8858,23 @@
       <c r="BL40" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="BM40" s="153"/>
-      <c r="BN40" s="153"/>
-      <c r="BO40" s="154"/>
-      <c r="BP40" s="154"/>
-      <c r="BQ40" s="154"/>
-      <c r="BR40" s="155"/>
-      <c r="BS40" s="152"/>
-      <c r="BT40" s="153"/>
-      <c r="BU40" s="154"/>
-      <c r="BV40" s="154"/>
-      <c r="BW40" s="154"/>
-      <c r="BX40" s="155"/>
+      <c r="BM40" s="125"/>
+      <c r="BN40" s="125"/>
+      <c r="BO40" s="126"/>
+      <c r="BP40" s="126"/>
+      <c r="BQ40" s="126"/>
+      <c r="BR40" s="127"/>
+      <c r="BS40" s="124"/>
+      <c r="BT40" s="125"/>
+      <c r="BU40" s="126"/>
+      <c r="BV40" s="126"/>
+      <c r="BW40" s="126"/>
+      <c r="BX40" s="127"/>
     </row>
     <row r="41" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="105"/>
-      <c r="B41" s="106"/>
-      <c r="C41" s="109"/>
+      <c r="A41" s="156"/>
+      <c r="B41" s="167"/>
+      <c r="C41" s="158"/>
       <c r="D41" s="46">
         <v>2</v>
       </c>
@@ -9058,23 +9058,23 @@
       <c r="BL41" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="BM41" s="153"/>
-      <c r="BN41" s="153"/>
-      <c r="BO41" s="154"/>
-      <c r="BP41" s="154"/>
-      <c r="BQ41" s="154"/>
-      <c r="BR41" s="155"/>
-      <c r="BS41" s="152"/>
-      <c r="BT41" s="153"/>
-      <c r="BU41" s="154"/>
-      <c r="BV41" s="154"/>
-      <c r="BW41" s="154"/>
-      <c r="BX41" s="155"/>
+      <c r="BM41" s="125"/>
+      <c r="BN41" s="125"/>
+      <c r="BO41" s="126"/>
+      <c r="BP41" s="126"/>
+      <c r="BQ41" s="126"/>
+      <c r="BR41" s="127"/>
+      <c r="BS41" s="124"/>
+      <c r="BT41" s="125"/>
+      <c r="BU41" s="126"/>
+      <c r="BV41" s="126"/>
+      <c r="BW41" s="126"/>
+      <c r="BX41" s="127"/>
     </row>
     <row r="42" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="105"/>
-      <c r="B42" s="106"/>
-      <c r="C42" s="110"/>
+      <c r="A42" s="156"/>
+      <c r="B42" s="167"/>
+      <c r="C42" s="159"/>
       <c r="D42" s="100">
         <v>3</v>
       </c>
@@ -9258,260 +9258,260 @@
       <c r="BL42" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="BM42" s="176"/>
-      <c r="BN42" s="176"/>
-      <c r="BO42" s="177"/>
-      <c r="BP42" s="177"/>
-      <c r="BQ42" s="177"/>
-      <c r="BR42" s="178"/>
-      <c r="BS42" s="175"/>
-      <c r="BT42" s="176"/>
-      <c r="BU42" s="177"/>
-      <c r="BV42" s="177"/>
-      <c r="BW42" s="177"/>
-      <c r="BX42" s="178"/>
+      <c r="BM42" s="148"/>
+      <c r="BN42" s="148"/>
+      <c r="BO42" s="149"/>
+      <c r="BP42" s="149"/>
+      <c r="BQ42" s="149"/>
+      <c r="BR42" s="150"/>
+      <c r="BS42" s="147"/>
+      <c r="BT42" s="148"/>
+      <c r="BU42" s="149"/>
+      <c r="BV42" s="149"/>
+      <c r="BW42" s="149"/>
+      <c r="BX42" s="150"/>
     </row>
     <row r="43" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="105"/>
-      <c r="B43" s="106"/>
-      <c r="C43" s="111" t="s">
+      <c r="A43" s="156"/>
+      <c r="B43" s="167"/>
+      <c r="C43" s="160" t="s">
         <v>46</v>
       </c>
       <c r="D43" s="45">
         <v>1</v>
       </c>
-      <c r="E43" s="169"/>
-      <c r="F43" s="170"/>
-      <c r="G43" s="170"/>
-      <c r="H43" s="170"/>
-      <c r="I43" s="170"/>
-      <c r="J43" s="171"/>
-      <c r="K43" s="172"/>
-      <c r="L43" s="169"/>
-      <c r="M43" s="170"/>
-      <c r="N43" s="170"/>
-      <c r="O43" s="170"/>
-      <c r="P43" s="171"/>
-      <c r="Q43" s="172"/>
-      <c r="R43" s="169"/>
-      <c r="S43" s="170"/>
-      <c r="T43" s="170"/>
-      <c r="U43" s="170"/>
-      <c r="V43" s="173"/>
-      <c r="W43" s="172"/>
-      <c r="X43" s="169"/>
-      <c r="Y43" s="170"/>
-      <c r="Z43" s="170"/>
-      <c r="AA43" s="170"/>
-      <c r="AB43" s="171"/>
-      <c r="AC43" s="172"/>
-      <c r="AD43" s="169"/>
-      <c r="AE43" s="170"/>
-      <c r="AF43" s="170"/>
-      <c r="AG43" s="170"/>
-      <c r="AH43" s="171"/>
-      <c r="AI43" s="172"/>
-      <c r="AJ43" s="169"/>
-      <c r="AK43" s="170"/>
-      <c r="AL43" s="170"/>
-      <c r="AM43" s="170"/>
-      <c r="AN43" s="171"/>
-      <c r="AO43" s="169"/>
-      <c r="AP43" s="170"/>
-      <c r="AQ43" s="170"/>
-      <c r="AR43" s="170"/>
-      <c r="AS43" s="170"/>
-      <c r="AT43" s="171"/>
-      <c r="AU43" s="172"/>
-      <c r="AV43" s="169"/>
-      <c r="AW43" s="170"/>
-      <c r="AX43" s="170"/>
-      <c r="AY43" s="170"/>
-      <c r="AZ43" s="171"/>
-      <c r="BA43" s="172"/>
-      <c r="BB43" s="169"/>
-      <c r="BC43" s="170"/>
-      <c r="BD43" s="170"/>
-      <c r="BE43" s="170"/>
-      <c r="BF43" s="173"/>
-      <c r="BG43" s="172"/>
-      <c r="BH43" s="169"/>
-      <c r="BI43" s="170"/>
-      <c r="BJ43" s="170"/>
-      <c r="BK43" s="170"/>
-      <c r="BL43" s="171"/>
-      <c r="BM43" s="172"/>
-      <c r="BN43" s="169"/>
-      <c r="BO43" s="170"/>
-      <c r="BP43" s="170"/>
-      <c r="BQ43" s="170"/>
-      <c r="BR43" s="171"/>
-      <c r="BS43" s="172"/>
-      <c r="BT43" s="169"/>
-      <c r="BU43" s="170"/>
-      <c r="BV43" s="170"/>
-      <c r="BW43" s="170"/>
-      <c r="BX43" s="171"/>
+      <c r="E43" s="141"/>
+      <c r="F43" s="142"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="142"/>
+      <c r="I43" s="142"/>
+      <c r="J43" s="143"/>
+      <c r="K43" s="144"/>
+      <c r="L43" s="141"/>
+      <c r="M43" s="142"/>
+      <c r="N43" s="142"/>
+      <c r="O43" s="142"/>
+      <c r="P43" s="143"/>
+      <c r="Q43" s="144"/>
+      <c r="R43" s="141"/>
+      <c r="S43" s="142"/>
+      <c r="T43" s="142"/>
+      <c r="U43" s="142"/>
+      <c r="V43" s="145"/>
+      <c r="W43" s="144"/>
+      <c r="X43" s="141"/>
+      <c r="Y43" s="142"/>
+      <c r="Z43" s="142"/>
+      <c r="AA43" s="142"/>
+      <c r="AB43" s="143"/>
+      <c r="AC43" s="144"/>
+      <c r="AD43" s="141"/>
+      <c r="AE43" s="142"/>
+      <c r="AF43" s="142"/>
+      <c r="AG43" s="142"/>
+      <c r="AH43" s="143"/>
+      <c r="AI43" s="144"/>
+      <c r="AJ43" s="141"/>
+      <c r="AK43" s="142"/>
+      <c r="AL43" s="142"/>
+      <c r="AM43" s="142"/>
+      <c r="AN43" s="143"/>
+      <c r="AO43" s="141"/>
+      <c r="AP43" s="142"/>
+      <c r="AQ43" s="142"/>
+      <c r="AR43" s="142"/>
+      <c r="AS43" s="142"/>
+      <c r="AT43" s="143"/>
+      <c r="AU43" s="144"/>
+      <c r="AV43" s="141"/>
+      <c r="AW43" s="142"/>
+      <c r="AX43" s="142"/>
+      <c r="AY43" s="142"/>
+      <c r="AZ43" s="143"/>
+      <c r="BA43" s="144"/>
+      <c r="BB43" s="141"/>
+      <c r="BC43" s="142"/>
+      <c r="BD43" s="142"/>
+      <c r="BE43" s="142"/>
+      <c r="BF43" s="145"/>
+      <c r="BG43" s="144"/>
+      <c r="BH43" s="141"/>
+      <c r="BI43" s="142"/>
+      <c r="BJ43" s="142"/>
+      <c r="BK43" s="142"/>
+      <c r="BL43" s="143"/>
+      <c r="BM43" s="144"/>
+      <c r="BN43" s="141"/>
+      <c r="BO43" s="142"/>
+      <c r="BP43" s="142"/>
+      <c r="BQ43" s="142"/>
+      <c r="BR43" s="143"/>
+      <c r="BS43" s="144"/>
+      <c r="BT43" s="141"/>
+      <c r="BU43" s="142"/>
+      <c r="BV43" s="142"/>
+      <c r="BW43" s="142"/>
+      <c r="BX43" s="143"/>
     </row>
     <row r="44" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="105"/>
-      <c r="B44" s="106"/>
-      <c r="C44" s="111"/>
+      <c r="A44" s="156"/>
+      <c r="B44" s="167"/>
+      <c r="C44" s="160"/>
       <c r="D44" s="46">
         <v>2</v>
       </c>
-      <c r="E44" s="158"/>
-      <c r="F44" s="159"/>
-      <c r="G44" s="159"/>
-      <c r="H44" s="159"/>
-      <c r="I44" s="159"/>
-      <c r="J44" s="160"/>
-      <c r="K44" s="157"/>
-      <c r="L44" s="158"/>
-      <c r="M44" s="159"/>
-      <c r="N44" s="159"/>
-      <c r="O44" s="159"/>
-      <c r="P44" s="160"/>
-      <c r="Q44" s="157"/>
-      <c r="R44" s="158"/>
-      <c r="S44" s="159"/>
-      <c r="T44" s="159"/>
-      <c r="U44" s="159"/>
-      <c r="V44" s="174"/>
-      <c r="W44" s="157"/>
-      <c r="X44" s="158"/>
-      <c r="Y44" s="159"/>
-      <c r="Z44" s="159"/>
-      <c r="AA44" s="159"/>
-      <c r="AB44" s="160"/>
-      <c r="AC44" s="157"/>
-      <c r="AD44" s="158"/>
-      <c r="AE44" s="159"/>
-      <c r="AF44" s="159"/>
-      <c r="AG44" s="159"/>
-      <c r="AH44" s="160"/>
-      <c r="AI44" s="157"/>
-      <c r="AJ44" s="158"/>
-      <c r="AK44" s="159"/>
-      <c r="AL44" s="159"/>
-      <c r="AM44" s="159"/>
-      <c r="AN44" s="160"/>
-      <c r="AO44" s="158"/>
-      <c r="AP44" s="159"/>
-      <c r="AQ44" s="159"/>
-      <c r="AR44" s="159"/>
-      <c r="AS44" s="159"/>
-      <c r="AT44" s="160"/>
-      <c r="AU44" s="157"/>
-      <c r="AV44" s="158"/>
-      <c r="AW44" s="159"/>
-      <c r="AX44" s="159"/>
-      <c r="AY44" s="159"/>
-      <c r="AZ44" s="160"/>
-      <c r="BA44" s="157"/>
-      <c r="BB44" s="158"/>
-      <c r="BC44" s="159"/>
-      <c r="BD44" s="159"/>
-      <c r="BE44" s="159"/>
-      <c r="BF44" s="174"/>
-      <c r="BG44" s="157"/>
-      <c r="BH44" s="158"/>
-      <c r="BI44" s="159"/>
-      <c r="BJ44" s="159"/>
-      <c r="BK44" s="159"/>
-      <c r="BL44" s="160"/>
-      <c r="BM44" s="157"/>
-      <c r="BN44" s="158"/>
-      <c r="BO44" s="159"/>
-      <c r="BP44" s="159"/>
-      <c r="BQ44" s="159"/>
-      <c r="BR44" s="160"/>
-      <c r="BS44" s="157"/>
-      <c r="BT44" s="158"/>
-      <c r="BU44" s="159"/>
-      <c r="BV44" s="159"/>
-      <c r="BW44" s="159"/>
-      <c r="BX44" s="160"/>
+      <c r="E44" s="130"/>
+      <c r="F44" s="131"/>
+      <c r="G44" s="131"/>
+      <c r="H44" s="131"/>
+      <c r="I44" s="131"/>
+      <c r="J44" s="132"/>
+      <c r="K44" s="129"/>
+      <c r="L44" s="130"/>
+      <c r="M44" s="131"/>
+      <c r="N44" s="131"/>
+      <c r="O44" s="131"/>
+      <c r="P44" s="132"/>
+      <c r="Q44" s="129"/>
+      <c r="R44" s="130"/>
+      <c r="S44" s="131"/>
+      <c r="T44" s="131"/>
+      <c r="U44" s="131"/>
+      <c r="V44" s="146"/>
+      <c r="W44" s="129"/>
+      <c r="X44" s="130"/>
+      <c r="Y44" s="131"/>
+      <c r="Z44" s="131"/>
+      <c r="AA44" s="131"/>
+      <c r="AB44" s="132"/>
+      <c r="AC44" s="129"/>
+      <c r="AD44" s="130"/>
+      <c r="AE44" s="131"/>
+      <c r="AF44" s="131"/>
+      <c r="AG44" s="131"/>
+      <c r="AH44" s="132"/>
+      <c r="AI44" s="129"/>
+      <c r="AJ44" s="130"/>
+      <c r="AK44" s="131"/>
+      <c r="AL44" s="131"/>
+      <c r="AM44" s="131"/>
+      <c r="AN44" s="132"/>
+      <c r="AO44" s="130"/>
+      <c r="AP44" s="131"/>
+      <c r="AQ44" s="131"/>
+      <c r="AR44" s="131"/>
+      <c r="AS44" s="131"/>
+      <c r="AT44" s="132"/>
+      <c r="AU44" s="129"/>
+      <c r="AV44" s="130"/>
+      <c r="AW44" s="131"/>
+      <c r="AX44" s="131"/>
+      <c r="AY44" s="131"/>
+      <c r="AZ44" s="132"/>
+      <c r="BA44" s="129"/>
+      <c r="BB44" s="130"/>
+      <c r="BC44" s="131"/>
+      <c r="BD44" s="131"/>
+      <c r="BE44" s="131"/>
+      <c r="BF44" s="146"/>
+      <c r="BG44" s="129"/>
+      <c r="BH44" s="130"/>
+      <c r="BI44" s="131"/>
+      <c r="BJ44" s="131"/>
+      <c r="BK44" s="131"/>
+      <c r="BL44" s="132"/>
+      <c r="BM44" s="129"/>
+      <c r="BN44" s="130"/>
+      <c r="BO44" s="131"/>
+      <c r="BP44" s="131"/>
+      <c r="BQ44" s="131"/>
+      <c r="BR44" s="132"/>
+      <c r="BS44" s="129"/>
+      <c r="BT44" s="130"/>
+      <c r="BU44" s="131"/>
+      <c r="BV44" s="131"/>
+      <c r="BW44" s="131"/>
+      <c r="BX44" s="132"/>
     </row>
     <row r="45" spans="1:79" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="105"/>
-      <c r="B45" s="106"/>
-      <c r="C45" s="112"/>
+      <c r="A45" s="156"/>
+      <c r="B45" s="167"/>
+      <c r="C45" s="164"/>
       <c r="D45" s="46">
         <v>3</v>
       </c>
-      <c r="E45" s="158"/>
-      <c r="F45" s="159"/>
-      <c r="G45" s="159"/>
-      <c r="H45" s="159"/>
-      <c r="I45" s="159"/>
-      <c r="J45" s="160"/>
-      <c r="K45" s="157"/>
-      <c r="L45" s="158"/>
-      <c r="M45" s="159"/>
-      <c r="N45" s="159"/>
-      <c r="O45" s="159"/>
-      <c r="P45" s="160"/>
-      <c r="Q45" s="157"/>
-      <c r="R45" s="158"/>
-      <c r="S45" s="159"/>
-      <c r="T45" s="159"/>
-      <c r="U45" s="159"/>
-      <c r="V45" s="174"/>
-      <c r="W45" s="157"/>
-      <c r="X45" s="158"/>
-      <c r="Y45" s="159"/>
-      <c r="Z45" s="159"/>
-      <c r="AA45" s="159"/>
-      <c r="AB45" s="160"/>
-      <c r="AC45" s="157"/>
-      <c r="AD45" s="158"/>
-      <c r="AE45" s="159"/>
-      <c r="AF45" s="159"/>
-      <c r="AG45" s="159"/>
-      <c r="AH45" s="160"/>
-      <c r="AI45" s="157"/>
-      <c r="AJ45" s="158"/>
-      <c r="AK45" s="159"/>
-      <c r="AL45" s="159"/>
-      <c r="AM45" s="159"/>
-      <c r="AN45" s="160"/>
-      <c r="AO45" s="158"/>
-      <c r="AP45" s="159"/>
-      <c r="AQ45" s="159"/>
-      <c r="AR45" s="159"/>
-      <c r="AS45" s="159"/>
-      <c r="AT45" s="160"/>
-      <c r="AU45" s="157"/>
-      <c r="AV45" s="158"/>
-      <c r="AW45" s="159"/>
-      <c r="AX45" s="159"/>
-      <c r="AY45" s="159"/>
-      <c r="AZ45" s="160"/>
-      <c r="BA45" s="157"/>
-      <c r="BB45" s="158"/>
-      <c r="BC45" s="159"/>
-      <c r="BD45" s="159"/>
-      <c r="BE45" s="159"/>
-      <c r="BF45" s="174"/>
-      <c r="BG45" s="157"/>
-      <c r="BH45" s="158"/>
-      <c r="BI45" s="159"/>
-      <c r="BJ45" s="159"/>
-      <c r="BK45" s="159"/>
-      <c r="BL45" s="160"/>
-      <c r="BM45" s="157"/>
-      <c r="BN45" s="158"/>
-      <c r="BO45" s="159"/>
-      <c r="BP45" s="159"/>
-      <c r="BQ45" s="159"/>
-      <c r="BR45" s="160"/>
-      <c r="BS45" s="157"/>
-      <c r="BT45" s="158"/>
-      <c r="BU45" s="159"/>
-      <c r="BV45" s="159"/>
-      <c r="BW45" s="159"/>
-      <c r="BX45" s="160"/>
+      <c r="E45" s="130"/>
+      <c r="F45" s="131"/>
+      <c r="G45" s="131"/>
+      <c r="H45" s="131"/>
+      <c r="I45" s="131"/>
+      <c r="J45" s="132"/>
+      <c r="K45" s="129"/>
+      <c r="L45" s="130"/>
+      <c r="M45" s="131"/>
+      <c r="N45" s="131"/>
+      <c r="O45" s="131"/>
+      <c r="P45" s="132"/>
+      <c r="Q45" s="129"/>
+      <c r="R45" s="130"/>
+      <c r="S45" s="131"/>
+      <c r="T45" s="131"/>
+      <c r="U45" s="131"/>
+      <c r="V45" s="146"/>
+      <c r="W45" s="129"/>
+      <c r="X45" s="130"/>
+      <c r="Y45" s="131"/>
+      <c r="Z45" s="131"/>
+      <c r="AA45" s="131"/>
+      <c r="AB45" s="132"/>
+      <c r="AC45" s="129"/>
+      <c r="AD45" s="130"/>
+      <c r="AE45" s="131"/>
+      <c r="AF45" s="131"/>
+      <c r="AG45" s="131"/>
+      <c r="AH45" s="132"/>
+      <c r="AI45" s="129"/>
+      <c r="AJ45" s="130"/>
+      <c r="AK45" s="131"/>
+      <c r="AL45" s="131"/>
+      <c r="AM45" s="131"/>
+      <c r="AN45" s="132"/>
+      <c r="AO45" s="130"/>
+      <c r="AP45" s="131"/>
+      <c r="AQ45" s="131"/>
+      <c r="AR45" s="131"/>
+      <c r="AS45" s="131"/>
+      <c r="AT45" s="132"/>
+      <c r="AU45" s="129"/>
+      <c r="AV45" s="130"/>
+      <c r="AW45" s="131"/>
+      <c r="AX45" s="131"/>
+      <c r="AY45" s="131"/>
+      <c r="AZ45" s="132"/>
+      <c r="BA45" s="129"/>
+      <c r="BB45" s="130"/>
+      <c r="BC45" s="131"/>
+      <c r="BD45" s="131"/>
+      <c r="BE45" s="131"/>
+      <c r="BF45" s="146"/>
+      <c r="BG45" s="129"/>
+      <c r="BH45" s="130"/>
+      <c r="BI45" s="131"/>
+      <c r="BJ45" s="131"/>
+      <c r="BK45" s="131"/>
+      <c r="BL45" s="132"/>
+      <c r="BM45" s="129"/>
+      <c r="BN45" s="130"/>
+      <c r="BO45" s="131"/>
+      <c r="BP45" s="131"/>
+      <c r="BQ45" s="131"/>
+      <c r="BR45" s="132"/>
+      <c r="BS45" s="129"/>
+      <c r="BT45" s="130"/>
+      <c r="BU45" s="131"/>
+      <c r="BV45" s="131"/>
+      <c r="BW45" s="131"/>
+      <c r="BX45" s="132"/>
     </row>
     <row r="46" spans="1:79" x14ac:dyDescent="0.5">
       <c r="A46" s="8"/>
@@ -9590,9 +9590,9 @@
       <c r="BV46" s="42"/>
       <c r="BW46" s="44"/>
       <c r="BX46" s="20"/>
-      <c r="BY46" s="179"/>
-      <c r="BZ46" s="179"/>
-      <c r="CA46" s="180"/>
+      <c r="BY46" s="151"/>
+      <c r="BZ46" s="151"/>
+      <c r="CA46" s="152"/>
     </row>
     <row r="47" spans="1:79" x14ac:dyDescent="0.5">
       <c r="A47" s="8"/>
@@ -9671,18 +9671,18 @@
       <c r="BV47" s="42"/>
       <c r="BW47" s="44"/>
       <c r="BX47" s="20"/>
-      <c r="BY47" s="179"/>
-      <c r="BZ47" s="179"/>
-      <c r="CA47" s="180"/>
+      <c r="BY47" s="151"/>
+      <c r="BZ47" s="151"/>
+      <c r="CA47" s="152"/>
     </row>
     <row r="48" spans="1:79" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="105" t="s">
+      <c r="A48" s="156" t="s">
         <v>427</v>
       </c>
-      <c r="B48" s="119" t="s">
+      <c r="B48" s="161" t="s">
         <v>447</v>
       </c>
-      <c r="C48" s="113" t="s">
+      <c r="C48" s="157" t="s">
         <v>45</v>
       </c>
       <c r="D48" s="84">
@@ -9810,9 +9810,9 @@
       <c r="BX48" s="73"/>
     </row>
     <row r="49" spans="1:76" x14ac:dyDescent="0.5">
-      <c r="A49" s="105"/>
-      <c r="B49" s="120"/>
-      <c r="C49" s="109"/>
+      <c r="A49" s="156"/>
+      <c r="B49" s="162"/>
+      <c r="C49" s="158"/>
       <c r="D49" s="84">
         <v>2</v>
       </c>
@@ -9938,9 +9938,9 @@
       <c r="BX49" s="73"/>
     </row>
     <row r="50" spans="1:76" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="105"/>
-      <c r="B50" s="120"/>
-      <c r="C50" s="110"/>
+      <c r="A50" s="156"/>
+      <c r="B50" s="162"/>
+      <c r="C50" s="159"/>
       <c r="D50" s="85">
         <v>3</v>
       </c>
@@ -10066,9 +10066,9 @@
       <c r="BX50" s="78"/>
     </row>
     <row r="51" spans="1:76" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="105"/>
-      <c r="B51" s="120"/>
-      <c r="C51" s="111" t="s">
+      <c r="A51" s="156"/>
+      <c r="B51" s="162"/>
+      <c r="C51" s="160" t="s">
         <v>46</v>
       </c>
       <c r="D51" s="45">
@@ -10148,9 +10148,9 @@
       <c r="BX51" s="82"/>
     </row>
     <row r="52" spans="1:76" x14ac:dyDescent="0.5">
-      <c r="A52" s="105"/>
-      <c r="B52" s="120"/>
-      <c r="C52" s="111"/>
+      <c r="A52" s="156"/>
+      <c r="B52" s="162"/>
+      <c r="C52" s="160"/>
       <c r="D52" s="46">
         <v>2</v>
       </c>
@@ -10228,8 +10228,8 @@
       <c r="BX52" s="73"/>
     </row>
     <row r="53" spans="1:76" x14ac:dyDescent="0.5">
-      <c r="A53" s="105"/>
-      <c r="B53" s="107"/>
+      <c r="A53" s="156"/>
+      <c r="B53" s="163"/>
       <c r="C53" s="98"/>
       <c r="D53" s="46">
         <v>3</v>
@@ -10309,6 +10309,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="BG1:BL1"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="AI1:AN1"/>
+    <mergeCell ref="AO1:AT1"/>
+    <mergeCell ref="AU1:AZ1"/>
+    <mergeCell ref="BA1:BF1"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="A3:A15"/>
+    <mergeCell ref="A18:A30"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="B25:B30"/>
     <mergeCell ref="BM1:BR1"/>
     <mergeCell ref="BS1:BX1"/>
     <mergeCell ref="A48:A53"/>
@@ -10325,27 +10346,6 @@
     <mergeCell ref="B33:B38"/>
     <mergeCell ref="B40:B45"/>
     <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A3:A15"/>
-    <mergeCell ref="A18:A30"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="K1:P1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="W1:AB1"/>
-    <mergeCell ref="AC1:AH1"/>
-    <mergeCell ref="AI1:AN1"/>
-    <mergeCell ref="AO1:AT1"/>
-    <mergeCell ref="AU1:AZ1"/>
-    <mergeCell ref="BA1:BF1"/>
-    <mergeCell ref="BG1:BL1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM33:AN45 AU39 AS39:AT45 BA39 AY39:AZ45 BG39 BK33:BL45 H40:H42 N40:N42 T40:T42 Z18:Z27 Z33:Z42 AF18:AF27 AF33:AF42 AL18:AL27 AL33:AL42 AR39:AR42 AX39:AX42 BD39:BD42 BJ33:BJ42 BP18:BP23 BV18:BV23 AA33:AB45 T18:V27 AM3:AN9 BG43:BG45 BA43:BA45 K43:K45 T33:V35 U39:V45 AA18:AB30 Q9 Z3:AB12 Q24 W9 K9 BG24 K24 Q43:Q45 AC9 AG3:AH9 W24 W43:W45 AI9 BW33:BX45 BQ18:BR30 BW3:BX9 AC43:AC45 AI43:AI45 BE3:BF9 BE39:BF45 BD33:BF35 BQ33:BR45 BW18:BX30 AY3:AZ9 BA9 AI24 BK3:BL9 BA24 BG9 AU9 AS3:AT9 AC24 AU24 AM18:AN30 BM39:BM45 BM9 BQ3:BR9 BM24 BS39:BS45 BS9 H3:J12 N3:P12 T3:V12 AR18:AT27 AX18:AZ27 BD18:BF27 BS24 H18:J27 N18:P27 AG18:AH30 BJ18:BL30 H33:J35 N33:P35 AG33:AH45 AR33:AT35 AX33:AZ35 I39:J45 K39 AU43:AU45 Q39 O39:P45 W39 AC39 AI39 AG48:AH52 BS53 BK53:BM53 BQ48:BR53 AG53:AI53 AC53 BW48:BX53 O53:Q53 U53:W53 I53:K53 H48:J50 N48:P50 T48:V50 AA48:AB53 AY53:BA53 BE48:BF50 BE53:BG53 AS48:AT50 AY48:AZ50 BK48:BL52 AM48:AN53 AS53:AU53 Z48:Z50" xr:uid="{E34F1815-20B7-49E3-AC65-05E343F9EBE9}">
@@ -10360,10 +10360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDC4D68-62E8-4DA9-94DA-C895A0937673}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -10372,56 +10372,60 @@
     <col min="3" max="4" width="18" style="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.5859375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.41015625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5859375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.29296875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1171875" style="1"/>
+    <col min="7" max="8" width="17.41015625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5859375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.29296875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="2" spans="1:9" s="64" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="121" t="s">
+    <row r="1" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="2" spans="1:10" s="64" customFormat="1" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="172" t="s">
         <v>388</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121" t="s">
+      <c r="B2" s="172"/>
+      <c r="C2" s="172" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="128" t="s">
+      <c r="D2" s="179" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="121" t="s">
+      <c r="E2" s="172" t="s">
         <v>394</v>
       </c>
-      <c r="F2" s="121" t="s">
+      <c r="F2" s="172" t="s">
         <v>389</v>
       </c>
-      <c r="G2" s="121" t="s">
+      <c r="G2" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="121" t="s">
+      <c r="H2" s="179" t="s">
+        <v>451</v>
+      </c>
+      <c r="I2" s="172" t="s">
         <v>391</v>
       </c>
-      <c r="I2" s="123" t="s">
+      <c r="J2" s="174" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="64" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="122"/>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="124"/>
+    <row r="3" spans="1:10" s="64" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="173"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="173"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="173"/>
+      <c r="F3" s="173"/>
+      <c r="G3" s="173"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="173"/>
+      <c r="J3" s="175"/>
     </row>
-    <row r="4" spans="1:9" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="125" t="s">
+    <row r="4" spans="1:10" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="176" t="s">
         <v>388</v>
       </c>
-      <c r="B4" s="121"/>
+      <c r="B4" s="172"/>
       <c r="C4" s="66" t="s">
         <v>382</v>
       </c>
@@ -10440,13 +10444,16 @@
       <c r="H4" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="62" t="s">
+      <c r="I4" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="126"/>
-      <c r="B5" s="105"/>
+    <row r="5" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="177"/>
+      <c r="B5" s="156"/>
       <c r="C5" s="65" t="s">
         <v>386</v>
       </c>
@@ -10465,13 +10472,16 @@
       <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="126"/>
-      <c r="B6" s="105"/>
+    <row r="6" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="177"/>
+      <c r="B6" s="156"/>
       <c r="C6" s="65" t="s">
         <v>383</v>
       </c>
@@ -10490,13 +10500,16 @@
       <c r="H6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="126"/>
-      <c r="B7" s="105"/>
+    <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="177"/>
+      <c r="B7" s="156"/>
       <c r="C7" s="65" t="s">
         <v>384</v>
       </c>
@@ -10515,13 +10528,16 @@
       <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="126"/>
-      <c r="B8" s="105"/>
+    <row r="8" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="177"/>
+      <c r="B8" s="156"/>
       <c r="C8" s="65" t="s">
         <v>385</v>
       </c>
@@ -10540,13 +10556,16 @@
       <c r="H8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="127"/>
-      <c r="B9" s="122"/>
+    <row r="9" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="178"/>
+      <c r="B9" s="173"/>
       <c r="C9" s="67" t="s">
         <v>387</v>
       </c>
@@ -10565,15 +10584,18 @@
       <c r="H9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="125" t="s">
+    <row r="10" spans="1:10" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="176" t="s">
         <v>392</v>
       </c>
-      <c r="B10" s="121"/>
+      <c r="B10" s="172"/>
       <c r="C10" s="66" t="s">
         <v>382</v>
       </c>
@@ -10592,13 +10614,16 @@
       <c r="H10" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="62" t="s">
+      <c r="I10" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="126"/>
-      <c r="B11" s="105"/>
+    <row r="11" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="177"/>
+      <c r="B11" s="156"/>
       <c r="C11" s="65" t="s">
         <v>386</v>
       </c>
@@ -10617,13 +10642,16 @@
       <c r="H11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="126"/>
-      <c r="B12" s="105"/>
+    <row r="12" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="177"/>
+      <c r="B12" s="156"/>
       <c r="C12" s="65" t="s">
         <v>383</v>
       </c>
@@ -10642,13 +10670,16 @@
       <c r="H12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="126"/>
-      <c r="B13" s="105"/>
+    <row r="13" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="177"/>
+      <c r="B13" s="156"/>
       <c r="C13" s="65" t="s">
         <v>384</v>
       </c>
@@ -10667,13 +10698,16 @@
       <c r="H13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="126"/>
-      <c r="B14" s="105"/>
+    <row r="14" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="177"/>
+      <c r="B14" s="156"/>
       <c r="C14" s="65" t="s">
         <v>385</v>
       </c>
@@ -10692,13 +10726,16 @@
       <c r="H14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="127"/>
-      <c r="B15" s="122"/>
+    <row r="15" spans="1:10" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="178"/>
+      <c r="B15" s="173"/>
       <c r="C15" s="67" t="s">
         <v>387</v>
       </c>
@@ -10717,15 +10754,18 @@
       <c r="H15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="125" t="s">
+    <row r="16" spans="1:10" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="176" t="s">
         <v>393</v>
       </c>
-      <c r="B16" s="121"/>
+      <c r="B16" s="172"/>
       <c r="C16" s="66" t="s">
         <v>382</v>
       </c>
@@ -10744,13 +10784,16 @@
       <c r="H16" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="62" t="s">
+      <c r="I16" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="126"/>
-      <c r="B17" s="105"/>
+    <row r="17" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="177"/>
+      <c r="B17" s="156"/>
       <c r="C17" s="65" t="s">
         <v>386</v>
       </c>
@@ -10769,13 +10812,16 @@
       <c r="H17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="126"/>
-      <c r="B18" s="105"/>
+    <row r="18" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="177"/>
+      <c r="B18" s="156"/>
       <c r="C18" s="65" t="s">
         <v>383</v>
       </c>
@@ -10794,13 +10840,16 @@
       <c r="H18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="126"/>
-      <c r="B19" s="105"/>
+    <row r="19" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="177"/>
+      <c r="B19" s="156"/>
       <c r="C19" s="65" t="s">
         <v>384</v>
       </c>
@@ -10819,13 +10868,16 @@
       <c r="H19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="126"/>
-      <c r="B20" s="105"/>
+    <row r="20" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="177"/>
+      <c r="B20" s="156"/>
       <c r="C20" s="65" t="s">
         <v>385</v>
       </c>
@@ -10844,13 +10896,16 @@
       <c r="H20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="127"/>
-      <c r="B21" s="122"/>
+    <row r="21" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="178"/>
+      <c r="B21" s="173"/>
       <c r="C21" s="67" t="s">
         <v>387</v>
       </c>
@@ -10869,16 +10924,19 @@
       <c r="H21" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.5"/>
+    <row r="22" spans="1:10" ht="14.7" thickTop="1" x14ac:dyDescent="0.5"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="A10:B15"/>
     <mergeCell ref="A16:B21"/>
     <mergeCell ref="D2:D3"/>
@@ -10887,6 +10945,7 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>